<commit_message>
Added description to ingredient table in excel file
</commit_message>
<xml_diff>
--- a/documentation/db_entries.xlsx
+++ b/documentation/db_entries.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\E-commerce\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3852"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>recipe</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>description</t>
   </si>
 </sst>
 </file>
@@ -426,20 +429,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -453,12 +456,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -474,13 +477,16 @@
       <c r="E16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -494,17 +500,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Added some entries to database. Updated newexample.php
</commit_message>
<xml_diff>
--- a/documentation/db_entries.xlsx
+++ b/documentation/db_entries.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\E-commerce\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3855"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="3852"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -729,12 +729,18 @@
       <name val="Inherit"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -750,7 +756,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -768,6 +774,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="12" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1085,18 +1098,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B208" sqref="B208"/>
+    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
+      <selection activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="38.28515625" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1"/>
+    <col min="2" max="2" width="38.33203125" customWidth="1"/>
     <col min="3" max="3" width="11" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1119,72 +1132,72 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="A3" s="9">
         <v>35382</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="10">
         <v>100</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="A4" s="9">
         <v>47024</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="10">
         <v>100</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5">
+      <c r="A5" s="9">
         <v>47319</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="10">
         <v>100</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="11" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6">
+      <c r="A6" s="9">
         <v>54384</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="10">
         <v>100</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="9" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7">
+      <c r="A7" s="9">
         <v>35171</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="10">
         <v>100</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="11" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1203,58 +1216,58 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
+      <c r="A9" s="9">
         <v>47746</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="10">
         <v>100</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="9" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
+      <c r="A10" s="9">
         <v>47899</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="10">
         <v>100</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="9" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
+      <c r="A11" s="9">
         <v>47042</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="10">
         <v>100</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="11" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12">
+      <c r="A12" s="9">
         <v>713134</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="9" t="s">
         <v>204</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="10">
         <v>100</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="9" t="s">
         <v>205</v>
       </c>
     </row>
@@ -1283,159 +1296,183 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
-      <c r="B17">
+    <row r="17" spans="1:6">
+      <c r="A17" s="9"/>
+      <c r="B17" s="9">
         <v>35382</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="10">
         <v>2</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F17" t="s">
+      <c r="E17" s="9"/>
+      <c r="F17" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
-      <c r="B18">
+    <row r="18" spans="1:6">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9">
         <v>35382</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="10">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="2:6">
-      <c r="B19">
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9">
         <v>35382</v>
       </c>
-      <c r="C19" s="4">
-        <v>1</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C19" s="10">
+        <v>1</v>
+      </c>
+      <c r="D19" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
-      <c r="B20">
+    <row r="20" spans="1:6">
+      <c r="A20" s="9"/>
+      <c r="B20" s="9">
         <v>35382</v>
       </c>
-      <c r="C20" s="4">
+      <c r="C20" s="10">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
-      <c r="B21">
+    <row r="21" spans="1:6">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9">
         <v>35382</v>
       </c>
-      <c r="C21" s="4">
+      <c r="C21" s="10">
         <v>0.5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="9" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
-      <c r="B22">
+    <row r="22" spans="1:6">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9">
         <v>35382</v>
       </c>
-      <c r="C22" s="4">
-        <v>1</v>
-      </c>
-      <c r="D22" t="s">
+      <c r="C22" s="10">
+        <v>1</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="9" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
-      <c r="B24">
+    <row r="23" spans="1:6">
+      <c r="A23" s="9"/>
+      <c r="B23" s="9"/>
+      <c r="C23" s="10"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9">
         <v>47024</v>
       </c>
-      <c r="C24" s="4">
-        <v>1</v>
-      </c>
-      <c r="D24" t="s">
+      <c r="C24" s="10">
+        <v>1</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="F24" t="s">
+      <c r="F24" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
-      <c r="B25">
+    <row r="25" spans="1:6">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9">
         <v>47024</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="10">
         <v>8</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E25" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="26" spans="2:6">
-      <c r="B26">
+      <c r="F25" s="9"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="9"/>
+      <c r="B26" s="9">
         <v>47024</v>
       </c>
-      <c r="D26" t="s">
+      <c r="C26" s="10"/>
+      <c r="D26" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="27" spans="2:6">
-      <c r="B27">
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9">
         <v>47024</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E27" t="s">
+      <c r="E27" s="9" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="2:6">
+      <c r="F27" s="9"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="B29">
         <v>47319</v>
       </c>
@@ -1452,7 +1489,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="1:6">
       <c r="B30">
         <v>47319</v>
       </c>
@@ -1466,7 +1503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="1:6">
       <c r="B31">
         <v>47319</v>
       </c>
@@ -1477,7 +1514,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="1:6">
       <c r="B32">
         <v>47319</v>
       </c>
@@ -2498,128 +2535,133 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="28.5">
-      <c r="A136">
+    <row r="136" spans="1:3" ht="27.6">
+      <c r="A136" s="9">
         <v>35382</v>
       </c>
-      <c r="B136" s="1" t="s">
+      <c r="B136" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="C136" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="57">
-      <c r="A137">
+      <c r="C136" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="55.2">
+      <c r="A137" s="9">
         <v>35382</v>
       </c>
-      <c r="B137" s="1" t="s">
+      <c r="B137" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="C137" s="4">
+      <c r="C137" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="57">
-      <c r="A138">
+    <row r="138" spans="1:3" ht="55.2">
+      <c r="A138" s="9">
         <v>35382</v>
       </c>
-      <c r="B138" s="1" t="s">
+      <c r="B138" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C138" s="4">
+      <c r="C138" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="42.75">
-      <c r="A139">
+    <row r="139" spans="1:3" ht="27.6">
+      <c r="A139" s="9">
         <v>35382</v>
       </c>
-      <c r="B139" s="1" t="s">
+      <c r="B139" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C139" s="4">
+      <c r="C139" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="114">
-      <c r="A140">
+    <row r="140" spans="1:3" ht="96.6">
+      <c r="A140" s="9">
         <v>35382</v>
       </c>
-      <c r="B140" s="1" t="s">
+      <c r="B140" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C140" s="4">
+      <c r="C140" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="28.5">
-      <c r="A141">
+    <row r="141" spans="1:3" ht="27.6">
+      <c r="A141" s="9">
         <v>35382</v>
       </c>
-      <c r="B141" s="1" t="s">
+      <c r="B141" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C141" s="4">
+      <c r="C141" s="10">
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="42.75">
-      <c r="A142">
+    <row r="142" spans="1:3" ht="41.4">
+      <c r="A142" s="9">
         <v>35382</v>
       </c>
-      <c r="B142" s="1" t="s">
+      <c r="B142" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C142" s="4">
+      <c r="C142" s="10">
         <v>7</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="15.75">
-      <c r="A144">
+    <row r="143" spans="1:3">
+      <c r="A143" s="9"/>
+      <c r="B143" s="9"/>
+      <c r="C143" s="10"/>
+    </row>
+    <row r="144" spans="1:3" ht="15.6">
+      <c r="A144" s="9">
         <v>47024</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B144" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C144" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="15.75">
-      <c r="A145">
+      <c r="C144" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" ht="15.6">
+      <c r="A145" s="9">
         <v>47024</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C145" s="4">
+      <c r="C145" s="10">
         <v>2</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="15.75">
-      <c r="A146">
+    <row r="146" spans="1:3" ht="15.6">
+      <c r="A146" s="9">
         <v>47024</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C146" s="4">
+      <c r="C146" s="10">
         <v>3</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="15.75">
-      <c r="A147">
+    <row r="147" spans="1:3" ht="15.6">
+      <c r="A147" s="9">
         <v>47024</v>
       </c>
-      <c r="B147" s="2" t="s">
+      <c r="B147" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C147" s="4">
+      <c r="C147" s="10">
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.75">
+    <row r="149" spans="1:3" ht="15.6">
       <c r="A149">
         <v>47319</v>
       </c>
@@ -2630,7 +2672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="15.75">
+    <row r="150" spans="1:3" ht="15.6">
       <c r="A150">
         <v>47319</v>
       </c>
@@ -2641,7 +2683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="15.75">
+    <row r="151" spans="1:3" ht="15.6">
       <c r="A151">
         <v>47319</v>
       </c>
@@ -2652,7 +2694,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15.75">
+    <row r="152" spans="1:3" ht="15.6">
       <c r="A152">
         <v>47319</v>
       </c>
@@ -2663,7 +2705,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="15.75">
+    <row r="153" spans="1:3" ht="15.6">
       <c r="A153">
         <v>47319</v>
       </c>
@@ -2718,7 +2760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="42.75">
+    <row r="160" spans="1:3" ht="27.6">
       <c r="A160">
         <v>35171</v>
       </c>
@@ -2729,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="85.5">
+    <row r="161" spans="1:3" ht="82.8">
       <c r="A161">
         <v>35171</v>
       </c>
@@ -2740,7 +2782,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="28.5">
+    <row r="162" spans="1:3" ht="27.6">
       <c r="A162">
         <v>35171</v>
       </c>
@@ -2751,7 +2793,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="42.75">
+    <row r="163" spans="1:3" ht="41.4">
       <c r="A163">
         <v>35171</v>
       </c>
@@ -2762,7 +2804,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="15.75">
+    <row r="165" spans="1:3" ht="15.6">
       <c r="A165" t="s">
         <v>115</v>
       </c>
@@ -2773,7 +2815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="15.75">
+    <row r="166" spans="1:3" ht="15.6">
       <c r="A166" t="s">
         <v>115</v>
       </c>
@@ -2784,7 +2826,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:3" ht="15.75">
+    <row r="167" spans="1:3" ht="15.6">
       <c r="A167" t="s">
         <v>115</v>
       </c>
@@ -2795,7 +2837,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="15.75">
+    <row r="168" spans="1:3" ht="15.6">
       <c r="A168" t="s">
         <v>115</v>
       </c>
@@ -2806,7 +2848,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="15.75">
+    <row r="169" spans="1:3" ht="15.6">
       <c r="A169" t="s">
         <v>115</v>
       </c>
@@ -2817,7 +2859,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="15.75">
+    <row r="170" spans="1:3" ht="15.6">
       <c r="A170" t="s">
         <v>115</v>
       </c>
@@ -2828,7 +2870,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="15.75">
+    <row r="171" spans="1:3" ht="15.6">
       <c r="A171" t="s">
         <v>115</v>
       </c>
@@ -2839,7 +2881,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="172" spans="1:3" ht="15.75">
+    <row r="172" spans="1:3" ht="15.6">
       <c r="A172" t="s">
         <v>115</v>
       </c>
@@ -2850,7 +2892,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="173" spans="1:3" ht="15.75">
+    <row r="173" spans="1:3" ht="15.6">
       <c r="A173" t="s">
         <v>115</v>
       </c>
@@ -2861,7 +2903,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="15.75">
+    <row r="174" spans="1:3" ht="15.6">
       <c r="A174" t="s">
         <v>115</v>
       </c>
@@ -2873,7 +2915,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="15" customHeight="1"/>
-    <row r="176" spans="1:3">
+    <row r="176" spans="1:3" ht="409.6">
       <c r="A176">
         <v>47746</v>
       </c>
@@ -3016,7 +3058,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.75">
+    <row r="191" spans="1:3" ht="15.6">
       <c r="A191">
         <v>47042</v>
       </c>
@@ -3027,7 +3069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:3" ht="15.75">
+    <row r="192" spans="1:3" ht="15.6">
       <c r="A192">
         <v>47042</v>
       </c>
@@ -3038,7 +3080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.75">
+    <row r="193" spans="1:3" ht="15.6">
       <c r="A193">
         <v>47042</v>
       </c>
@@ -3049,7 +3091,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.75">
+    <row r="194" spans="1:3" ht="15.6">
       <c r="A194">
         <v>47042</v>
       </c>
@@ -3060,7 +3102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.75">
+    <row r="195" spans="1:3" ht="15.6">
       <c r="A195">
         <v>47042</v>
       </c>
@@ -3071,7 +3113,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.75">
+    <row r="196" spans="1:3" ht="15.6">
       <c r="A196">
         <v>47042</v>
       </c>
@@ -3082,7 +3124,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15.75">
+    <row r="197" spans="1:3" ht="15.6">
       <c r="A197">
         <v>47042</v>
       </c>
@@ -3151,8 +3193,11 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D8" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D7" r:id="rId3"/>
+    <hyperlink ref="D11" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added more entries to db
</commit_message>
<xml_diff>
--- a/documentation/db_entries.xlsx
+++ b/documentation/db_entries.xlsx
@@ -356,18 +356,6 @@
     <t>room temperature, grated</t>
   </si>
   <si>
-    <t>1. Mix the chicken, hot sauce, mayo, carrot, celery and onion in a small bowl.</t>
-  </si>
-  <si>
-    <t>2. Butter the outside of each slice of bread, sprinkle half of the cheeses on the inside of one slice of bread, top with the buffalo chicken salad, the remaining cheese and finally the other slice of bread.</t>
-  </si>
-  <si>
-    <t>3. Heat a non-stick pan over medium heat.</t>
-  </si>
-  <si>
-    <t>4. Add the sandwich and grill until golden brown and the cheese has melted, about 2-4 minutes per side.</t>
-  </si>
-  <si>
     <t>Cinnamon Rolls</t>
   </si>
   <si>
@@ -494,9 +482,6 @@
     <t>cold</t>
   </si>
   <si>
-    <t>1. Stir together the flour, salt, and instant yeast in a 4-quart bowl (or in the bowl of an electric mixer). With a large metal spoon, stir in the oil and the cold water until the flour is all absorbed (or mix on low speed with the paddle attachment), If you are mixing by hand, repeatedly dip one of your hands or the metal spoon into cold water and use it, much like a dough hook, to work the dough vigorously into a smooth mass while rotating the bowl in a circular motion with the other hand. Reverse the circular motion a few times to develop the gluten further. Do this for 5 to 7 minutes, or until the dough is smooth and the ingredients are evenly distributed. If you are using an electric mixer, switch to the dough hook and mix on medium speed for 5 to 7 minutes, or as long as it takes to create a smooth, sticky dough. The dough should clear the sides of the bowl but stick to the bottom of the bowl. If the dough is too wet and doesn't come off the sides of the bowl, sprinkle in some more flour just until it clears the sides. If it clears the bottom of the bowl, dribble in a tea- spoon or two of cold water. The finished dough will be springy, elastic, and sticky, not just tacky, and register 50 to 55F.</t>
-  </si>
-  <si>
     <t>2. Sprinkle flour on the counter and transfer the dough to the counter. Prepare a sheet pan by lining it with baking parchment and misting the parchment with spray oil (or lightly oil the parchment). Using a metal dough scraper, cut the dough into 6 equal pieces (or larger if you are comfortable shaping large pizzas), You can dip the scraper into the water between cuts to keep the dough from sticking to it, Sprinkle flour over the dough. Make sure your hands are dry and then flour them. Lift each piece and gently round it into a ball. If the dough sticks to your hands, dip your hands into the flour again. Transfer the dough balls to the sheet pan, Mist the dough generously with spray oil and slip the pan into a food-grade plastic bag.</t>
   </si>
   <si>
@@ -672,6 +657,21 @@
   </si>
   <si>
     <t>5. Season with an little dusting of sea salt and extra parmesan cheese and serve.</t>
+  </si>
+  <si>
+    <t>Add the sandwich and grill until golden brown and the cheese has melted, about 2-4 minutes per side.</t>
+  </si>
+  <si>
+    <t>Heat a non-stick pan over medium heat.</t>
+  </si>
+  <si>
+    <t>Butter the outside of each slice of bread, sprinkle half of the cheeses on the inside of one slice of bread, top with the buffalo chicken salad, the remaining cheese and finally the other slice of bread.</t>
+  </si>
+  <si>
+    <t>Mix the chicken, hot sauce, mayo, carrot, celery and onion in a small bowl.</t>
+  </si>
+  <si>
+    <t>Stir together the flour, salt, and instant yeast in a 4-quart bowl (or in the bowl of an electric mixer). With a large metal spoon, stir in the oil and the cold water until the flour is all absorbed (or mix on low speed with the paddle attachment), If you are mixing by hand, repeatedly dip one of your hands or the metal spoon into cold water and use it, much like a dough hook, to work the dough vigorously into a smooth mass while rotating the bowl in a circular motion wi+B156th the other hand. Reverse the circular motion a few times to develop the gluten further. Do this for 5 to 7 minutes, or until the dough is smooth and the ingredients are evenly distributed. If you are using an electric mixer, switch to the dough hook and mix on medium speed for 5 to 7 minutes, or as long as it takes to create a smooth, sticky dough. The dough should clear the sides of the bowl but stick to the bottom of the bowl. If the dough is too wet and doesn't come off the sides of the bowl, sprinkle in some more flour just until it clears the sides. If it clears the bottom of the bowl, dribble in a tea- spoon or two of cold water. The finished dough will be springy, elastic, and sticky, not just tacky, and register 50 to 55F.</t>
   </si>
 </sst>
 </file>
@@ -756,15 +756,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -781,6 +775,11 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1098,17 +1097,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="D138" sqref="D138"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="38.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" customWidth="1"/>
-    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1124,7 +1123,7 @@
       <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" t="s">
@@ -1132,143 +1131,143 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9">
+      <c r="A3" s="7">
         <v>35382</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="8">
         <v>100</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="7" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9">
+      <c r="A4" s="7">
         <v>47024</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="8">
         <v>100</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9">
+      <c r="A5" s="7">
         <v>47319</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="8">
         <v>100</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="9" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9">
+      <c r="A6" s="7">
         <v>54384</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="8">
         <v>100</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="9">
+      <c r="A7" s="7">
         <v>35171</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="10">
+      <c r="C7" s="8">
         <v>100</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>114</v>
-      </c>
-      <c r="C8" s="4">
+        <v>110</v>
+      </c>
+      <c r="C8" s="2">
         <v>100</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>116</v>
+      <c r="D8" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="9">
+      <c r="A9" s="7">
         <v>47746</v>
       </c>
-      <c r="B9" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="10">
+      <c r="B9" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9" s="8">
         <v>100</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>147</v>
+      <c r="D9" s="7" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="9">
+      <c r="A10" s="7">
         <v>47899</v>
       </c>
-      <c r="B10" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="B10" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="C10" s="8">
         <v>100</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>166</v>
+      <c r="D10" s="7" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="9">
+      <c r="A11" s="7">
         <v>47042</v>
       </c>
-      <c r="B11" s="9" t="s">
-        <v>186</v>
-      </c>
-      <c r="C11" s="10">
+      <c r="B11" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="C11" s="8">
         <v>100</v>
       </c>
-      <c r="D11" s="11" t="s">
-        <v>187</v>
+      <c r="D11" s="9" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="9">
+      <c r="A12" s="7">
         <v>713134</v>
       </c>
-      <c r="B12" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="C12" s="10">
+      <c r="B12" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="8">
         <v>100</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>205</v>
+      <c r="D12" s="7" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1283,7 +1282,7 @@
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D16" t="s">
@@ -1297,621 +1296,727 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="9"/>
-      <c r="B17" s="9">
+      <c r="A17" s="7">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7">
         <v>35382</v>
       </c>
-      <c r="C17" s="10">
+      <c r="C17" s="8">
         <v>2</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9" t="s">
+      <c r="E17" s="7"/>
+      <c r="F17" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="9"/>
-      <c r="B18" s="9">
+      <c r="A18" s="7">
+        <v>5</v>
+      </c>
+      <c r="B18" s="7">
         <v>35382</v>
       </c>
-      <c r="C18" s="10">
+      <c r="C18" s="8">
         <v>2</v>
       </c>
-      <c r="D18" s="9" t="s">
+      <c r="D18" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="9"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="9"/>
-      <c r="B19" s="9">
+      <c r="A19" s="7">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7">
         <v>35382</v>
       </c>
-      <c r="C19" s="10">
-        <v>1</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="C19" s="8">
+        <v>1</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="9"/>
-      <c r="B20" s="9">
+      <c r="A20" s="7">
+        <v>7</v>
+      </c>
+      <c r="B20" s="7">
         <v>35382</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="8">
         <v>2</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D20" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="9" t="s">
+      <c r="E20" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="7" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="9"/>
-      <c r="B21" s="9">
+      <c r="A21" s="7">
+        <v>8</v>
+      </c>
+      <c r="B21" s="7">
         <v>35382</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="8">
         <v>0.5</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D21" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="9" t="s">
+      <c r="F21" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="9"/>
-      <c r="B22" s="9">
+      <c r="A22" s="7">
+        <v>9</v>
+      </c>
+      <c r="B22" s="7">
         <v>35382</v>
       </c>
-      <c r="C22" s="10">
-        <v>1</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="C22" s="8">
+        <v>1</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="9" t="s">
+      <c r="E22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="9"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="9"/>
-      <c r="B24" s="9">
+      <c r="A24" s="7">
+        <v>0</v>
+      </c>
+      <c r="B24" s="7">
         <v>47024</v>
       </c>
-      <c r="C24" s="10">
-        <v>1</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="9" t="s">
+      <c r="E24" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="F24" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="9"/>
-      <c r="B25" s="9">
+      <c r="A25" s="7">
+        <v>1</v>
+      </c>
+      <c r="B25" s="7">
         <v>47024</v>
       </c>
-      <c r="C25" s="10">
+      <c r="C25" s="8">
         <v>8</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D25" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="9" t="s">
+      <c r="E25" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" s="7"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="9"/>
-      <c r="B26" s="9">
+      <c r="A26" s="7">
+        <v>2</v>
+      </c>
+      <c r="B26" s="7">
         <v>47024</v>
       </c>
-      <c r="C26" s="10"/>
-      <c r="D26" s="9" t="s">
+      <c r="C26" s="8"/>
+      <c r="D26" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="9" t="s">
+      <c r="E26" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" s="7"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9">
+      <c r="A27" s="7">
+        <v>3</v>
+      </c>
+      <c r="B27" s="7">
         <v>47024</v>
       </c>
-      <c r="C27" s="10" t="s">
+      <c r="C27" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="9" t="s">
+      <c r="D27" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="9" t="s">
+      <c r="E27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="9"/>
-    </row>
-    <row r="29" spans="1:6">
-      <c r="B29">
+      <c r="F27" s="7"/>
+    </row>
+    <row r="29" spans="1:6" s="7" customFormat="1">
+      <c r="A29" s="7">
+        <v>10</v>
+      </c>
+      <c r="B29" s="7">
         <v>47319</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="8">
         <v>12</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E29" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="F29" t="s">
+      <c r="F29" s="7" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
-      <c r="B30">
+    <row r="30" spans="1:6" s="7" customFormat="1">
+      <c r="A30" s="7">
+        <v>11</v>
+      </c>
+      <c r="B30" s="7">
         <v>47319</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="8">
         <v>3</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E30" t="s">
+      <c r="E30" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
-      <c r="B31">
+    <row r="31" spans="1:6" s="7" customFormat="1">
+      <c r="A31" s="7">
+        <v>12</v>
+      </c>
+      <c r="B31" s="7">
         <v>47319</v>
       </c>
-      <c r="D31" t="s">
+      <c r="C31" s="8"/>
+      <c r="D31" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F31" t="s">
+      <c r="F31" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
-      <c r="B32">
+    <row r="32" spans="1:6" s="7" customFormat="1">
+      <c r="A32" s="7">
+        <v>13</v>
+      </c>
+      <c r="B32" s="7">
         <v>47319</v>
       </c>
-      <c r="D32" t="s">
+      <c r="C32" s="8"/>
+      <c r="D32" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F32" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="2:6">
-      <c r="B33">
+    <row r="33" spans="1:6" s="7" customFormat="1">
+      <c r="A33" s="7">
+        <v>14</v>
+      </c>
+      <c r="B33" s="7">
         <v>47319</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C33" s="8"/>
+      <c r="D33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F33" t="s">
+      <c r="F33" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="2:6">
-      <c r="B35">
+    <row r="34" spans="1:6" s="12" customFormat="1">
+      <c r="C34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" s="7" customFormat="1">
+      <c r="A35" s="7">
+        <v>15</v>
+      </c>
+      <c r="B35" s="7">
         <v>54384</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="8">
         <v>10</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E35" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F35" t="s">
+      <c r="F35" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="2:6">
-      <c r="B36">
+    <row r="36" spans="1:6" s="7" customFormat="1">
+      <c r="A36" s="7">
+        <v>16</v>
+      </c>
+      <c r="B36" s="7">
         <v>54384</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="8">
         <v>2</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F36" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="2:6">
-      <c r="B37">
+    <row r="37" spans="1:6" s="7" customFormat="1">
+      <c r="A37" s="7">
+        <v>17</v>
+      </c>
+      <c r="B37" s="7">
         <v>54384</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="8">
         <v>2</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F37" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="2:6">
-      <c r="B38">
+    <row r="38" spans="1:6" s="7" customFormat="1">
+      <c r="A38" s="7">
+        <v>18</v>
+      </c>
+      <c r="B38" s="7">
         <v>54384</v>
       </c>
-      <c r="C38" s="4">
+      <c r="C38" s="8">
         <v>2</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="E38" t="s">
+      <c r="E38" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="2:6">
-      <c r="B39">
+    <row r="39" spans="1:6" s="7" customFormat="1">
+      <c r="A39" s="7">
+        <v>19</v>
+      </c>
+      <c r="B39" s="7">
         <v>54384</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="8">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F39" s="7" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
-      <c r="B40">
+    <row r="40" spans="1:6" s="7" customFormat="1">
+      <c r="A40" s="7">
+        <v>20</v>
+      </c>
+      <c r="B40" s="7">
         <v>54384</v>
       </c>
-      <c r="D40" t="s">
+      <c r="C40" s="8"/>
+      <c r="D40" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
-      <c r="B41">
+    <row r="41" spans="1:6" s="7" customFormat="1">
+      <c r="A41" s="7">
+        <v>6</v>
+      </c>
+      <c r="B41" s="7">
         <v>54384</v>
       </c>
-      <c r="C41" s="4">
+      <c r="C41" s="8">
         <v>2</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="2:6">
-      <c r="B42">
+    <row r="42" spans="1:6" s="7" customFormat="1">
+      <c r="A42" s="7">
+        <v>21</v>
+      </c>
+      <c r="B42" s="7">
         <v>54384</v>
       </c>
-      <c r="C42" s="4">
+      <c r="C42" s="8">
         <v>2</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="2:6">
-      <c r="B43">
+    <row r="43" spans="1:6" s="7" customFormat="1">
+      <c r="A43" s="7">
+        <v>22</v>
+      </c>
+      <c r="B43" s="7">
         <v>54384</v>
       </c>
-      <c r="C43" s="4">
-        <v>1</v>
-      </c>
-      <c r="D43" t="s">
+      <c r="C43" s="8">
+        <v>1</v>
+      </c>
+      <c r="D43" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E43" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="2:6">
-      <c r="B44">
+    <row r="44" spans="1:6" s="7" customFormat="1">
+      <c r="A44" s="7">
+        <v>23</v>
+      </c>
+      <c r="B44" s="7">
         <v>54384</v>
       </c>
-      <c r="C44" s="4">
+      <c r="C44" s="8">
         <v>2</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="E44" t="s">
+      <c r="E44" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F44" t="s">
+      <c r="F44" s="7" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="2:6">
-      <c r="B45">
+    <row r="45" spans="1:6" s="7" customFormat="1">
+      <c r="A45" s="7">
+        <v>17</v>
+      </c>
+      <c r="B45" s="7">
         <v>54384</v>
       </c>
-      <c r="D45" t="s">
+      <c r="C45" s="8"/>
+      <c r="D45" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F45" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="2:6">
-      <c r="B47">
+    <row r="47" spans="1:6" s="7" customFormat="1">
+      <c r="A47" s="7">
+        <v>24</v>
+      </c>
+      <c r="B47" s="7">
         <v>35171</v>
       </c>
-      <c r="C47" s="4">
+      <c r="C47" s="8">
         <v>0.25</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E47" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F47" s="7" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="2:6">
-      <c r="B48">
+    <row r="48" spans="1:6" s="7" customFormat="1">
+      <c r="A48" s="7">
+        <v>25</v>
+      </c>
+      <c r="B48" s="7">
         <v>35171</v>
       </c>
-      <c r="C48" s="4">
-        <v>1</v>
-      </c>
-      <c r="D48" t="s">
+      <c r="C48" s="8">
+        <v>1</v>
+      </c>
+      <c r="D48" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="E48" t="s">
+      <c r="E48" s="7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="2:6">
-      <c r="B49">
+    <row r="49" spans="1:6" s="7" customFormat="1">
+      <c r="A49" s="7">
+        <v>26</v>
+      </c>
+      <c r="B49" s="7">
         <v>35171</v>
       </c>
-      <c r="C49" s="4">
+      <c r="C49" s="8">
         <v>0.5</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="E49" t="s">
+      <c r="E49" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F49" t="s">
+      <c r="F49" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="2:6">
-      <c r="B50">
+    <row r="50" spans="1:6" s="7" customFormat="1">
+      <c r="A50" s="7">
+        <v>27</v>
+      </c>
+      <c r="B50" s="7">
         <v>35171</v>
       </c>
-      <c r="C50" s="4">
-        <v>1</v>
-      </c>
-      <c r="D50" t="s">
+      <c r="C50" s="8">
+        <v>1</v>
+      </c>
+      <c r="D50" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E50" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F50" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="2:6">
-      <c r="B51">
+    <row r="51" spans="1:6" s="7" customFormat="1">
+      <c r="A51" s="7">
+        <v>28</v>
+      </c>
+      <c r="B51" s="7">
         <v>35171</v>
       </c>
-      <c r="C51" s="4">
-        <v>1</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="C51" s="8">
+        <v>1</v>
+      </c>
+      <c r="D51" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F51" s="7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="2:6">
-      <c r="B52">
+    <row r="52" spans="1:6" s="7" customFormat="1">
+      <c r="A52" s="7">
+        <v>29</v>
+      </c>
+      <c r="B52" s="7">
         <v>35171</v>
       </c>
-      <c r="C52" s="4">
-        <v>1</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="C52" s="8">
+        <v>1</v>
+      </c>
+      <c r="D52" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="E52" t="s">
+      <c r="E52" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F52" t="s">
+      <c r="F52" s="7" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="2:6">
-      <c r="B53">
+    <row r="53" spans="1:6" s="7" customFormat="1">
+      <c r="A53" s="7">
+        <v>30</v>
+      </c>
+      <c r="B53" s="7">
         <v>35171</v>
       </c>
-      <c r="C53" s="4">
-        <v>1</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="C53" s="8">
+        <v>1</v>
+      </c>
+      <c r="D53" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="E53" t="s">
+      <c r="E53" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F53" s="7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="2:6">
-      <c r="B54">
+    <row r="54" spans="1:6" s="7" customFormat="1">
+      <c r="A54" s="7">
+        <v>8</v>
+      </c>
+      <c r="B54" s="7">
         <v>35171</v>
       </c>
-      <c r="C54" s="4">
+      <c r="C54" s="8">
         <v>0.5</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="E54" t="s">
+      <c r="E54" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="7" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="2:6">
-      <c r="B55">
+    <row r="55" spans="1:6" s="7" customFormat="1">
+      <c r="A55" s="7">
+        <v>31</v>
+      </c>
+      <c r="B55" s="7">
         <v>35171</v>
       </c>
-      <c r="C55" s="4">
+      <c r="C55" s="8">
         <v>2</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E55" t="s">
+      <c r="E55" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="2:6">
-      <c r="B56">
+    <row r="56" spans="1:6" s="7" customFormat="1">
+      <c r="A56" s="7">
+        <v>6</v>
+      </c>
+      <c r="B56" s="7">
         <v>35171</v>
       </c>
-      <c r="C56" s="4">
-        <v>1</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="C56" s="8">
+        <v>1</v>
+      </c>
+      <c r="D56" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E56" t="s">
+      <c r="E56" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F56" t="s">
+      <c r="F56" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="58" spans="2:6">
+    <row r="58" spans="1:6">
       <c r="B58" t="s">
-        <v>115</v>
-      </c>
-      <c r="C58" s="4">
+        <v>111</v>
+      </c>
+      <c r="C58" s="2">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E58" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
       <c r="B59" t="s">
-        <v>115</v>
-      </c>
-      <c r="C59" s="4">
+        <v>111</v>
+      </c>
+      <c r="C59" s="2">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="2:6">
+    <row r="60" spans="1:6">
       <c r="B60" t="s">
+        <v>111</v>
+      </c>
+      <c r="C60" s="2">
+        <v>1</v>
+      </c>
+      <c r="D60" t="s">
         <v>115</v>
-      </c>
-      <c r="C60" s="4">
-        <v>1</v>
-      </c>
-      <c r="D60" t="s">
-        <v>119</v>
       </c>
       <c r="E60" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="61" spans="2:6">
+    <row r="61" spans="1:6">
       <c r="B61" t="s">
-        <v>115</v>
-      </c>
-      <c r="C61" s="4">
+        <v>111</v>
+      </c>
+      <c r="C61" s="2">
         <v>0.5</v>
       </c>
       <c r="D61" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E61" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="B62" t="s">
-        <v>115</v>
-      </c>
-      <c r="C62" s="4">
+        <v>111</v>
+      </c>
+      <c r="C62" s="2">
         <v>8</v>
       </c>
       <c r="D62" t="s">
@@ -1921,43 +2026,43 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="2:6">
+    <row r="63" spans="1:6">
       <c r="B63" t="s">
-        <v>115</v>
-      </c>
-      <c r="C63" s="4">
+        <v>111</v>
+      </c>
+      <c r="C63" s="2">
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E63" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
       <c r="B64" t="s">
-        <v>115</v>
-      </c>
-      <c r="C64" s="4">
+        <v>111</v>
+      </c>
+      <c r="C64" s="2">
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E64" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65" t="s">
-        <v>115</v>
-      </c>
-      <c r="C65" s="4">
+        <v>111</v>
+      </c>
+      <c r="C65" s="2">
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E65" t="s">
         <v>26</v>
@@ -1965,24 +2070,24 @@
     </row>
     <row r="66" spans="2:6">
       <c r="B66" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D66" t="s">
+        <v>125</v>
+      </c>
+      <c r="E66" t="s">
         <v>129</v>
-      </c>
-      <c r="E66" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="67" spans="2:6">
       <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" s="2">
+        <v>2</v>
+      </c>
+      <c r="D67" t="s">
         <v>115</v>
-      </c>
-      <c r="C67" s="4">
-        <v>2</v>
-      </c>
-      <c r="D67" t="s">
-        <v>119</v>
       </c>
       <c r="E67" t="s">
         <v>85</v>
@@ -1990,56 +2095,56 @@
     </row>
     <row r="68" spans="2:6">
       <c r="B68" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D68" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E68" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="69" spans="2:6">
       <c r="B69" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D69" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="70" spans="2:6">
       <c r="B70" t="s">
-        <v>115</v>
-      </c>
-      <c r="C70" s="4">
+        <v>111</v>
+      </c>
+      <c r="C70" s="2">
         <v>1</v>
       </c>
       <c r="D70" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E70" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="71" spans="2:6">
       <c r="B71" t="s">
-        <v>115</v>
-      </c>
-      <c r="C71" s="4">
+        <v>111</v>
+      </c>
+      <c r="C71" s="2">
         <v>2</v>
       </c>
       <c r="D71" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E71" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="72" spans="2:6">
       <c r="B72" t="s">
-        <v>115</v>
-      </c>
-      <c r="C72" s="4">
+        <v>111</v>
+      </c>
+      <c r="C72" s="2">
         <v>0.5</v>
       </c>
       <c r="D72" t="s">
@@ -2051,13 +2156,13 @@
     </row>
     <row r="73" spans="2:6">
       <c r="B73" t="s">
-        <v>115</v>
-      </c>
-      <c r="C73" s="4">
+        <v>111</v>
+      </c>
+      <c r="C73" s="2">
         <v>0.25</v>
       </c>
       <c r="D73" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E73" t="s">
         <v>27</v>
@@ -2065,13 +2170,13 @@
     </row>
     <row r="74" spans="2:6">
       <c r="B74" t="s">
-        <v>115</v>
-      </c>
-      <c r="C74" s="4">
+        <v>111</v>
+      </c>
+      <c r="C74" s="2">
         <v>0.25</v>
       </c>
       <c r="D74" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E74" t="s">
         <v>27</v>
@@ -2079,24 +2184,24 @@
     </row>
     <row r="75" spans="2:6">
       <c r="B75" t="s">
-        <v>115</v>
-      </c>
-      <c r="C75" s="4">
+        <v>111</v>
+      </c>
+      <c r="C75" s="2">
         <v>0.125</v>
       </c>
       <c r="D75" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E75" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="77" spans="2:6">
       <c r="B77">
         <v>47746</v>
       </c>
-      <c r="C77" s="4" t="s">
-        <v>149</v>
+      <c r="C77" s="2" t="s">
+        <v>145</v>
       </c>
       <c r="D77" t="s">
         <v>77</v>
@@ -2109,35 +2214,35 @@
       <c r="B78">
         <v>47746</v>
       </c>
-      <c r="C78" s="4" t="s">
-        <v>150</v>
+      <c r="C78" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D78" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E78" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="2:6">
       <c r="B79">
         <v>47746</v>
       </c>
-      <c r="C79" s="4">
+      <c r="C79" s="2">
         <v>1</v>
       </c>
       <c r="D79" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E79" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="80" spans="2:6">
       <c r="B80">
         <v>47746</v>
       </c>
-      <c r="C80" s="4">
+      <c r="C80" s="2">
         <v>0.25</v>
       </c>
       <c r="D80" t="s">
@@ -2154,17 +2259,17 @@
       <c r="B81">
         <v>47746</v>
       </c>
-      <c r="C81" s="4" t="s">
-        <v>150</v>
+      <c r="C81" s="2" t="s">
+        <v>146</v>
       </c>
       <c r="D81" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E81" t="s">
         <v>85</v>
       </c>
       <c r="F81" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="82" spans="2:6">
@@ -2172,21 +2277,21 @@
         <v>47746</v>
       </c>
       <c r="D82" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="F82" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="2:6">
       <c r="B84">
         <v>47899</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84" s="2">
         <v>0.5</v>
       </c>
       <c r="D84" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E84" t="s">
         <v>27</v>
@@ -2196,84 +2301,84 @@
       <c r="B85">
         <v>47899</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="2">
         <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E85" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="86" spans="2:6">
       <c r="B86">
         <v>47899</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86" s="2">
         <v>1</v>
       </c>
       <c r="D86" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E86" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87" spans="2:6">
       <c r="B87">
         <v>47899</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87" s="2">
         <v>1</v>
       </c>
       <c r="D87" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E87" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="2:6">
       <c r="B88">
         <v>47899</v>
       </c>
-      <c r="C88" s="4">
+      <c r="C88" s="2">
         <v>2</v>
       </c>
       <c r="D88" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E88" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="89" spans="2:6">
       <c r="B89">
         <v>47899</v>
       </c>
-      <c r="C89" s="4">
+      <c r="C89" s="2">
         <v>2</v>
       </c>
       <c r="D89" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="F89" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="90" spans="2:6">
       <c r="B90">
         <v>47899</v>
       </c>
-      <c r="C90" s="4">
+      <c r="C90" s="2">
         <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="F90" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="2:6">
@@ -2281,38 +2386,38 @@
         <v>47899</v>
       </c>
       <c r="D91" t="s">
+        <v>168</v>
+      </c>
+      <c r="E91" t="s">
         <v>173</v>
-      </c>
-      <c r="E91" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="92" spans="2:6">
       <c r="B92">
         <v>47899</v>
       </c>
-      <c r="C92" s="4">
+      <c r="C92" s="2">
         <v>0.25</v>
       </c>
       <c r="D92" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E92" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F92" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="93" spans="2:6">
       <c r="B93">
         <v>47899</v>
       </c>
-      <c r="C93" s="4">
+      <c r="C93" s="2">
         <v>1</v>
       </c>
       <c r="D93" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E93" t="s">
         <v>26</v>
@@ -2322,11 +2427,11 @@
       <c r="B95">
         <v>47042</v>
       </c>
-      <c r="C95" s="4">
+      <c r="C95" s="2">
         <v>1</v>
       </c>
       <c r="D95" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E95" t="s">
         <v>57</v>
@@ -2336,56 +2441,56 @@
       <c r="B96">
         <v>47042</v>
       </c>
-      <c r="C96" s="4">
+      <c r="C96" s="2">
         <v>1</v>
       </c>
       <c r="D96" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E96" t="s">
         <v>57</v>
       </c>
       <c r="F96" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="2:6">
       <c r="B97">
         <v>47042</v>
       </c>
-      <c r="C97" s="4">
+      <c r="C97" s="2">
         <v>1</v>
       </c>
       <c r="D97" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E97" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
     </row>
     <row r="98" spans="2:6">
       <c r="B98">
         <v>47042</v>
       </c>
-      <c r="C98" s="4">
+      <c r="C98" s="2">
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E98" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
     </row>
     <row r="99" spans="2:6">
       <c r="B99">
         <v>47042</v>
       </c>
-      <c r="C99" s="4">
+      <c r="C99" s="2">
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E99" t="s">
         <v>84</v>
@@ -2396,18 +2501,18 @@
         <v>47042</v>
       </c>
       <c r="D100" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
     </row>
     <row r="102" spans="2:6">
       <c r="B102">
         <v>713134</v>
       </c>
-      <c r="C102" s="4">
+      <c r="C102" s="2">
         <v>4</v>
       </c>
       <c r="D102" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E102" t="s">
         <v>85</v>
@@ -2417,11 +2522,11 @@
       <c r="B103">
         <v>713134</v>
       </c>
-      <c r="C103" s="4">
+      <c r="C103" s="2">
         <v>3</v>
       </c>
       <c r="D103" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E103" t="s">
         <v>84</v>
@@ -2431,67 +2536,67 @@
       <c r="B104">
         <v>713134</v>
       </c>
-      <c r="C104" s="4">
+      <c r="C104" s="2">
         <v>0.5</v>
       </c>
       <c r="D104" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E104" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="2:6">
       <c r="B105">
         <v>713134</v>
       </c>
-      <c r="C105" s="4">
+      <c r="C105" s="2">
         <v>0.5</v>
       </c>
       <c r="D105" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E105" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="106" spans="2:6">
       <c r="B106">
         <v>713134</v>
       </c>
-      <c r="C106" s="4">
+      <c r="C106" s="2">
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E106" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="107" spans="2:6">
       <c r="B107">
         <v>713134</v>
       </c>
-      <c r="C107" s="4">
+      <c r="C107" s="2">
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E107" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="2:6">
       <c r="B108">
         <v>713134</v>
       </c>
-      <c r="C108" s="4">
+      <c r="C108" s="2">
         <v>4</v>
       </c>
       <c r="D108" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E108" t="s">
         <v>84</v>
@@ -2512,7 +2617,7 @@
       <c r="B121" t="s">
         <v>6</v>
       </c>
-      <c r="C121" s="4" t="s">
+      <c r="C121" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D121" t="s">
@@ -2531,386 +2636,386 @@
       <c r="B135" t="s">
         <v>14</v>
       </c>
-      <c r="C135" s="4" t="s">
+      <c r="C135" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="136" spans="1:3" ht="27.6">
-      <c r="A136" s="9">
+      <c r="A136" s="7">
         <v>35382</v>
       </c>
-      <c r="B136" s="12" t="s">
+      <c r="B136" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C136" s="10">
+      <c r="C136" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="55.2">
-      <c r="A137" s="9">
+      <c r="A137" s="7">
         <v>35382</v>
       </c>
-      <c r="B137" s="12" t="s">
+      <c r="B137" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C137" s="10">
+      <c r="C137" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="138" spans="1:3" ht="55.2">
-      <c r="A138" s="9">
+      <c r="A138" s="7">
         <v>35382</v>
       </c>
-      <c r="B138" s="12" t="s">
+      <c r="B138" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C138" s="10">
+      <c r="C138" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="139" spans="1:3" ht="27.6">
-      <c r="A139" s="9">
+      <c r="A139" s="7">
         <v>35382</v>
       </c>
-      <c r="B139" s="12" t="s">
+      <c r="B139" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C139" s="10">
+      <c r="C139" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="140" spans="1:3" ht="96.6">
-      <c r="A140" s="9">
+      <c r="A140" s="7">
         <v>35382</v>
       </c>
-      <c r="B140" s="12" t="s">
+      <c r="B140" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C140" s="10">
+      <c r="C140" s="8">
         <v>5</v>
       </c>
     </row>
     <row r="141" spans="1:3" ht="27.6">
-      <c r="A141" s="9">
+      <c r="A141" s="7">
         <v>35382</v>
       </c>
-      <c r="B141" s="12" t="s">
+      <c r="B141" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C141" s="10">
+      <c r="C141" s="8">
         <v>6</v>
       </c>
     </row>
     <row r="142" spans="1:3" ht="41.4">
-      <c r="A142" s="9">
+      <c r="A142" s="7">
         <v>35382</v>
       </c>
-      <c r="B142" s="12" t="s">
+      <c r="B142" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C142" s="10">
+      <c r="C142" s="8">
         <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="9"/>
-      <c r="B143" s="9"/>
-      <c r="C143" s="10"/>
+      <c r="A143" s="7"/>
+      <c r="B143" s="7"/>
+      <c r="C143" s="8"/>
     </row>
     <row r="144" spans="1:3" ht="15.6">
-      <c r="A144" s="9">
+      <c r="A144" s="7">
         <v>47024</v>
       </c>
-      <c r="B144" s="13" t="s">
+      <c r="B144" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C144" s="10">
+      <c r="C144" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.6">
-      <c r="A145" s="9">
+      <c r="A145" s="7">
         <v>47024</v>
       </c>
-      <c r="B145" s="13" t="s">
+      <c r="B145" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="C145" s="10">
+      <c r="C145" s="8">
         <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.6">
-      <c r="A146" s="9">
+      <c r="A146" s="7">
         <v>47024</v>
       </c>
-      <c r="B146" s="13" t="s">
+      <c r="B146" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="C146" s="10">
+      <c r="C146" s="8">
         <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="15.6">
-      <c r="A147" s="9">
+      <c r="A147" s="7">
         <v>47024</v>
       </c>
-      <c r="B147" s="13" t="s">
+      <c r="B147" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C147" s="10">
+      <c r="C147" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:3" ht="15.6">
-      <c r="A149">
+    <row r="149" spans="1:3" s="7" customFormat="1" ht="15.6">
+      <c r="A149" s="7">
         <v>47319</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B149" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C149" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" ht="15.6">
-      <c r="A150">
+      <c r="C149" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" s="7" customFormat="1" ht="15.6">
+      <c r="A150" s="7">
         <v>47319</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="B150" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C150" s="4">
+      <c r="C150" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="15.6">
-      <c r="A151">
+    <row r="151" spans="1:3" s="7" customFormat="1" ht="15.6">
+      <c r="A151" s="7">
         <v>47319</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B151" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C151" s="4">
+      <c r="C151" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="15.6">
-      <c r="A152">
+    <row r="152" spans="1:3" s="7" customFormat="1" ht="15.6">
+      <c r="A152" s="7">
         <v>47319</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C152" s="4">
+      <c r="C152" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" ht="15.6">
-      <c r="A153">
+    <row r="153" spans="1:3" s="7" customFormat="1" ht="15.6">
+      <c r="A153" s="7">
         <v>47319</v>
       </c>
-      <c r="B153" s="2" t="s">
+      <c r="B153" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C153" s="4">
+      <c r="C153" s="8">
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A155">
+    <row r="155" spans="1:3" s="7" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A155" s="7">
         <v>54384</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B155" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="C155" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A156">
+      <c r="C155" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" s="7" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A156" s="7">
         <v>54384</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B156" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C156" s="4">
+      <c r="C156" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A157">
+    <row r="157" spans="1:3" s="7" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A157" s="7">
         <v>54384</v>
       </c>
-      <c r="B157" s="3" t="s">
+      <c r="B157" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C157" s="4">
+      <c r="C157" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="20.25" customHeight="1">
-      <c r="A158">
+    <row r="158" spans="1:3" s="7" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A158" s="7">
         <v>54384</v>
       </c>
-      <c r="B158" s="3" t="s">
+      <c r="B158" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="C158" s="4">
+      <c r="C158" s="8">
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:3" ht="27.6">
-      <c r="A160">
+    <row r="160" spans="1:3" s="7" customFormat="1" ht="41.4">
+      <c r="A160" s="7">
         <v>35171</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C160" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" ht="82.8">
-      <c r="A161">
+      <c r="B160" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="C160" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" s="7" customFormat="1" ht="82.8">
+      <c r="A161" s="7">
         <v>35171</v>
       </c>
-      <c r="B161" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C161" s="4">
+      <c r="B161" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="C161" s="8">
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" ht="27.6">
-      <c r="A162">
+    <row r="162" spans="1:3" s="7" customFormat="1" ht="27.6">
+      <c r="A162" s="7">
         <v>35171</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C162" s="4">
+      <c r="B162" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C162" s="8">
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="41.4">
-      <c r="A163">
+    <row r="163" spans="1:3" s="7" customFormat="1" ht="41.4">
+      <c r="A163" s="7">
         <v>35171</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C163" s="4">
+      <c r="B163" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="C163" s="8">
         <v>4</v>
       </c>
     </row>
     <row r="165" spans="1:3" ht="15.6">
       <c r="A165" t="s">
-        <v>115</v>
-      </c>
-      <c r="B165" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C165" s="4">
+        <v>111</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C165" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:3" ht="15.6">
       <c r="A166" t="s">
-        <v>115</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C166" s="4">
+        <v>111</v>
+      </c>
+      <c r="B166" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C166" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="15.6">
       <c r="A167" t="s">
-        <v>115</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C167" s="4">
+        <v>111</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C167" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="15.6">
       <c r="A168" t="s">
-        <v>115</v>
-      </c>
-      <c r="B168" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="C168" s="4">
+        <v>111</v>
+      </c>
+      <c r="B168" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C168" s="2">
         <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="15.6">
       <c r="A169" t="s">
-        <v>115</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C169" s="4">
+        <v>111</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C169" s="2">
         <v>5</v>
       </c>
     </row>
     <row r="170" spans="1:3" ht="15.6">
       <c r="A170" t="s">
-        <v>115</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C170" s="4">
+        <v>111</v>
+      </c>
+      <c r="B170" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C170" s="2">
         <v>6</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="15.6">
       <c r="A171" t="s">
-        <v>115</v>
-      </c>
-      <c r="B171" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C171" s="4">
+        <v>111</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C171" s="2">
         <v>7</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="15.6">
       <c r="A172" t="s">
-        <v>115</v>
-      </c>
-      <c r="B172" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="C172" s="4">
+        <v>111</v>
+      </c>
+      <c r="B172" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C172" s="2">
         <v>8</v>
       </c>
     </row>
     <row r="173" spans="1:3" ht="15.6">
       <c r="A173" t="s">
-        <v>115</v>
-      </c>
-      <c r="B173" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="C173" s="4">
+        <v>111</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C173" s="2">
         <v>9</v>
       </c>
     </row>
     <row r="174" spans="1:3" ht="15.6">
       <c r="A174" t="s">
-        <v>115</v>
-      </c>
-      <c r="B174" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="C174" s="4">
+        <v>111</v>
+      </c>
+      <c r="B174" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C174" s="2">
         <v>10</v>
       </c>
     </row>
@@ -2919,10 +3024,10 @@
       <c r="A176">
         <v>47746</v>
       </c>
-      <c r="B176" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C176" s="4">
+      <c r="B176" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="C176" s="2">
         <v>1</v>
       </c>
     </row>
@@ -2930,10 +3035,10 @@
       <c r="A177">
         <v>47746</v>
       </c>
-      <c r="B177" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="C177" s="4">
+      <c r="B177" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C177" s="2">
         <v>2</v>
       </c>
     </row>
@@ -2941,10 +3046,10 @@
       <c r="A178">
         <v>47746</v>
       </c>
-      <c r="B178" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="C178" s="4">
+      <c r="B178" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="C178" s="2">
         <v>3</v>
       </c>
     </row>
@@ -2952,10 +3057,10 @@
       <c r="A179">
         <v>47746</v>
       </c>
-      <c r="B179" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C179" s="4">
+      <c r="B179" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C179" s="2">
         <v>4</v>
       </c>
     </row>
@@ -2963,10 +3068,10 @@
       <c r="A180">
         <v>47746</v>
       </c>
-      <c r="B180" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="C180" s="4">
+      <c r="B180" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C180" s="2">
         <v>5</v>
       </c>
     </row>
@@ -2974,10 +3079,10 @@
       <c r="A181">
         <v>47746</v>
       </c>
-      <c r="B181" s="6" t="s">
-        <v>161</v>
-      </c>
-      <c r="C181" s="4">
+      <c r="B181" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C181" s="2">
         <v>6</v>
       </c>
     </row>
@@ -2985,10 +3090,10 @@
       <c r="A182">
         <v>47746</v>
       </c>
-      <c r="B182" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="C182" s="4">
+      <c r="B182" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C182" s="2">
         <v>7</v>
       </c>
     </row>
@@ -2996,10 +3101,10 @@
       <c r="A183">
         <v>47746</v>
       </c>
-      <c r="B183" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="C183" s="4">
+      <c r="B183" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C183" s="2">
         <v>8</v>
       </c>
     </row>
@@ -3007,10 +3112,10 @@
       <c r="A184">
         <v>47746</v>
       </c>
-      <c r="B184" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="C184" s="4">
+      <c r="B184" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C184" s="2">
         <v>9</v>
       </c>
     </row>
@@ -3018,10 +3123,10 @@
       <c r="A186">
         <v>47899</v>
       </c>
-      <c r="B186" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="C186" s="4">
+      <c r="B186" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C186" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3029,10 +3134,10 @@
       <c r="A187">
         <v>47899</v>
       </c>
-      <c r="B187" s="7" t="s">
-        <v>183</v>
-      </c>
-      <c r="C187" s="4">
+      <c r="B187" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="C187" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3040,10 +3145,10 @@
       <c r="A188">
         <v>47899</v>
       </c>
-      <c r="B188" s="7" t="s">
-        <v>184</v>
-      </c>
-      <c r="C188" s="4">
+      <c r="B188" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C188" s="2">
         <v>3</v>
       </c>
     </row>
@@ -3051,10 +3156,10 @@
       <c r="A189">
         <v>47899</v>
       </c>
-      <c r="B189" s="7" t="s">
-        <v>185</v>
-      </c>
-      <c r="C189" s="4">
+      <c r="B189" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C189" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3062,10 +3167,10 @@
       <c r="A191">
         <v>47042</v>
       </c>
-      <c r="B191" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="C191" s="4">
+      <c r="B191" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C191" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3073,10 +3178,10 @@
       <c r="A192">
         <v>47042</v>
       </c>
-      <c r="B192" s="2" t="s">
-        <v>198</v>
-      </c>
-      <c r="C192" s="4">
+      <c r="B192" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C192" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3084,10 +3189,10 @@
       <c r="A193">
         <v>47042</v>
       </c>
-      <c r="B193" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C193" s="4">
+      <c r="B193" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C193" s="2">
         <v>3</v>
       </c>
     </row>
@@ -3095,10 +3200,10 @@
       <c r="A194">
         <v>47042</v>
       </c>
-      <c r="B194" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="C194" s="4">
+      <c r="B194" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C194" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3106,10 +3211,10 @@
       <c r="A195">
         <v>47042</v>
       </c>
-      <c r="B195" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C195" s="4">
+      <c r="B195" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C195" s="2">
         <v>5</v>
       </c>
     </row>
@@ -3117,10 +3222,10 @@
       <c r="A196">
         <v>47042</v>
       </c>
-      <c r="B196" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C196" s="4">
+      <c r="B196" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="C196" s="2">
         <v>6</v>
       </c>
     </row>
@@ -3128,10 +3233,10 @@
       <c r="A197">
         <v>47042</v>
       </c>
-      <c r="B197" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="C197" s="4">
+      <c r="B197" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C197" s="2">
         <v>7</v>
       </c>
     </row>
@@ -3139,10 +3244,10 @@
       <c r="A199">
         <v>713134</v>
       </c>
-      <c r="B199" s="8" t="s">
-        <v>211</v>
-      </c>
-      <c r="C199" s="4">
+      <c r="B199" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="C199" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3150,10 +3255,10 @@
       <c r="A200">
         <v>713134</v>
       </c>
-      <c r="B200" s="8" t="s">
-        <v>212</v>
-      </c>
-      <c r="C200" s="4">
+      <c r="B200" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="C200" s="2">
         <v>2</v>
       </c>
     </row>
@@ -3161,10 +3266,10 @@
       <c r="A201">
         <v>713134</v>
       </c>
-      <c r="B201" s="8" t="s">
-        <v>213</v>
-      </c>
-      <c r="C201" s="4">
+      <c r="B201" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="C201" s="2">
         <v>3</v>
       </c>
     </row>
@@ -3172,10 +3277,10 @@
       <c r="A202">
         <v>713134</v>
       </c>
-      <c r="B202" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="C202" s="4">
+      <c r="B202" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C202" s="2">
         <v>4</v>
       </c>
     </row>
@@ -3183,10 +3288,10 @@
       <c r="A203">
         <v>713134</v>
       </c>
-      <c r="B203" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="C203" s="4">
+      <c r="B203" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C203" s="2">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added ingredient excel file to documentation folder
</commit_message>
<xml_diff>
--- a/documentation/db_entries.xlsx
+++ b/documentation/db_entries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="215">
   <si>
     <t>recipe</t>
   </si>
@@ -482,30 +482,6 @@
     <t>cold</t>
   </si>
   <si>
-    <t>2. Sprinkle flour on the counter and transfer the dough to the counter. Prepare a sheet pan by lining it with baking parchment and misting the parchment with spray oil (or lightly oil the parchment). Using a metal dough scraper, cut the dough into 6 equal pieces (or larger if you are comfortable shaping large pizzas), You can dip the scraper into the water between cuts to keep the dough from sticking to it, Sprinkle flour over the dough. Make sure your hands are dry and then flour them. Lift each piece and gently round it into a ball. If the dough sticks to your hands, dip your hands into the flour again. Transfer the dough balls to the sheet pan, Mist the dough generously with spray oil and slip the pan into a food-grade plastic bag.</t>
-  </si>
-  <si>
-    <t>3. Put the pan into the refrigerator overnight to rest the dough, or keep for up to 3 days. (Note: If you want to save some of the dough for future baking, you can store the dough balls in a zippered freezer bag. Dip each dough ball into a bowl that has a few tablespoons of oil in it, rolling the dough in the oil, and then put each ball into a separate bag. You can place the bags into the freezer for up to 3 months. Transfer them to the refrigerator the day before you plan to make pizza.)</t>
-  </si>
-  <si>
-    <t>4. On the day you plan to make the pizza, remove the desired number of dough balls from the refrigerator 2 hours before making the pizza. Before letting the dough rest at room temperature for 2 hours, dust the counter with flour, and then mist the counter with spray oil. Place the dough balls on top of the floured counter and sprinkle them with flour; dust your hands with flour. Gently press the dough into flat disks about 1/2 inch thick and 5 inches in diameter. Sprinkle the dough with flour, mist it again with spray oil, and cover the dough loosely with plastic wrap or a food-grade plastic bag. Now let rest for 2 hours.</t>
-  </si>
-  <si>
-    <t>5. At least 45 minutes before making the pizza, place a baking stone either on the floor of the oven (for gas ovens), or on a rack in the lower third of the oven. Heat the oven as hot as possible, up to 800F (most home ovens will go only to 500 to 550F, but some will go higher). If you do not have a baking stone, you can use the back of a sheet pan, but do not preheat the pan.</t>
-  </si>
-  <si>
-    <t>6. Generously dust a peel or the back of a sheet pan with semolina flour or cornmeal. Make the pizzas one at a time. Dip your hands, including the backs of your hands and knuckles, in flour and lift I piece of dough by getting under it with a pastry scraper. Very gently lay the dough across your fists and carefully stretch it by bouncing the dough in a circular motion on your hands, carefully giving it a little stretch with each bounce. If it begins to stick to your hands, lay it down on the floured counter and reflour your hands, then continue shaping it. Once the dough has expanded outward, move to a full toss as shown on page 208. If you have trouble tossing the dough, or if the dough keeps springing back, let it rest for 5 to 20 minutes so the gluten can relax, and try again. You can also resort to using a rolling pin, though this isn't as effective as the toss method.</t>
-  </si>
-  <si>
-    <t>7. When the dough is stretched out to your satisfaction (about 9 to 12 inches in diameter for a 6-ounce piece of dough), lay it on the peel or pan, making sure there is enough semolina flour or cornmeal to allow it to slide. Lightly top it with sauce and then with your other top- pings, remembering that the best pizzas are topped with a less-is-more philosophy. The American "kitchen sink" approach is counterproductive, as it makes the crust more difficult to bake. A few, usually no more than 3 or 4 toppings, including sauce and cheese is sufficient.</t>
-  </si>
-  <si>
-    <t>8. Slide the topped pizza onto the stone (or bake directly on the sheet pan) and close the door. Wait 2 minutes, then take a peek. If it needs to be rotated 180 degrees for even baking, do so. The pizza should take about 5 to 8 minutes to bake. If the top gets done before the bottom, you will need to move the stone to a lower self before the next round. if the bottom crisps before the cheese caramelizes, then you will need to raise the stone for subsequent bakes.</t>
-  </si>
-  <si>
-    <t>9. Remove the pizza from the oven and transfer to a cutting board. Wait 3 to 5 minutes before slicing and serving, to allow the cheese to set slightly</t>
-  </si>
-  <si>
     <t>Magic Sauce</t>
   </si>
   <si>
@@ -644,21 +620,6 @@
     <t>parmeshan cheese</t>
   </si>
   <si>
-    <t>1. Preheat your oven to 425 degrees.</t>
-  </si>
-  <si>
-    <t>2. Place the cubed potatoes onto a sprayed baking sheet or parchment lined baking dish dish.</t>
-  </si>
-  <si>
-    <t>3. Pile on the olive oil, garlic salt, salt, paprika, pepper and Parmesan cheese. Using your fingers, or a spoon if you feel inclined, toss the potatoes and carefully mix everything around until the seasonings coat each potato.</t>
-  </si>
-  <si>
-    <t>4. Transfer the baking vessel into the oven and bake for 15 minutes. Remove from the oven and toss the potatoes with a pair of tongs. Put the baking dish back into the oven and bake for 10 minutes more. Remove the baking sheet and give them another toss and place them back in the oven and roast until they are golden and crispy.</t>
-  </si>
-  <si>
-    <t>5. Season with an little dusting of sea salt and extra parmesan cheese and serve.</t>
-  </si>
-  <si>
     <t>Add the sandwich and grill until golden brown and the cheese has melted, about 2-4 minutes per side.</t>
   </si>
   <si>
@@ -671,7 +632,43 @@
     <t>Mix the chicken, hot sauce, mayo, carrot, celery and onion in a small bowl.</t>
   </si>
   <si>
-    <t>Stir together the flour, salt, and instant yeast in a 4-quart bowl (or in the bowl of an electric mixer). With a large metal spoon, stir in the oil and the cold water until the flour is all absorbed (or mix on low speed with the paddle attachment), If you are mixing by hand, repeatedly dip one of your hands or the metal spoon into cold water and use it, much like a dough hook, to work the dough vigorously into a smooth mass while rotating the bowl in a circular motion wi+B156th the other hand. Reverse the circular motion a few times to develop the gluten further. Do this for 5 to 7 minutes, or until the dough is smooth and the ingredients are evenly distributed. If you are using an electric mixer, switch to the dough hook and mix on medium speed for 5 to 7 minutes, or as long as it takes to create a smooth, sticky dough. The dough should clear the sides of the bowl but stick to the bottom of the bowl. If the dough is too wet and doesn't come off the sides of the bowl, sprinkle in some more flour just until it clears the sides. If it clears the bottom of the bowl, dribble in a tea- spoon or two of cold water. The finished dough will be springy, elastic, and sticky, not just tacky, and register 50 to 55F.</t>
+    <t>Preheat your oven to 425 degrees.</t>
+  </si>
+  <si>
+    <t>Place the cubed potatoes onto a sprayed baking sheet or parchment lined baking dish dish.</t>
+  </si>
+  <si>
+    <t>Pile on the olive oil, garlic salt, salt, paprika, pepper and Parmesan cheese. Using your fingers, or a spoon if you feel inclined, toss the potatoes and carefully mix everything around until the seasonings coat each potato.</t>
+  </si>
+  <si>
+    <t>Transfer the baking vessel into the oven and bake for 15 minutes. Remove from the oven and toss the potatoes with a pair of tongs. Put the baking dish back into the oven and bake for 10 minutes more. Remove the baking sheet and give them another toss and place them back in the oven and roast until they are golden and crispy.</t>
+  </si>
+  <si>
+    <t>Season with an little dusting of sea salt and extra parmesan cheese and serve.</t>
+  </si>
+  <si>
+    <t>Sprinkle flour on the counter and transfer the dough to the counter. Prepare a sheet pan by lining it with baking parchment and misting the parchment with spray oil (or lightly oil the parchment). Using a metal dough scraper, cut the dough into 6 equal pieces (or larger if you are comfortable shaping large pizzas), You can dip the scraper into the water between cuts to keep the dough from sticking to it, Sprinkle flour over the dough. Make sure your hands are dry and then flour them. Lift each piece and gently round it into a ball. If the dough sticks to your hands, dip your hands into the flour again. Transfer the dough balls to the sheet pan, Mist the dough generously with spray oil and slip the pan into a food-grade plastic bag.</t>
+  </si>
+  <si>
+    <t>Put the pan into the refrigerator overnight to rest the dough, or keep for up to 3 days. (Note: If you want to save some of the dough for future baking, you can store the dough balls in a zippered freezer bag. Dip each dough ball into a bowl that has a few tablespoons of oil in it, rolling the dough in the oil, and then put each ball into a separate bag. You can place the bags into the freezer for up to 3 months. Transfer them to the refrigerator the day before you plan to make pizza.)</t>
+  </si>
+  <si>
+    <t>On the day you plan to make the pizza, remove the desired number of dough balls from the refrigerator 2 hours before making the pizza. Before letting the dough rest at room temperature for 2 hours, dust the counter with flour, and then mist the counter with spray oil. Place the dough balls on top of the floured counter and sprinkle them with flour; dust your hands with flour. Gently press the dough into flat disks about 1/2 inch thick and 5 inches in diameter. Sprinkle the dough with flour, mist it again with spray oil, and cover the dough loosely with plastic wrap or a food-grade plastic bag. Now let rest for 2 hours.</t>
+  </si>
+  <si>
+    <t>At least 45 minutes before making the pizza, place a baking stone either on the floor of the oven (for gas ovens), or on a rack in the lower third of the oven. Heat the oven as hot as possible, up to 800F (most home ovens will go only to 500 to 550F, but some will go higher). If you do not have a baking stone, you can use the back of a sheet pan, but do not preheat the pan.</t>
+  </si>
+  <si>
+    <t>Generously dust a peel or the back of a sheet pan with semolina flour or cornmeal. Make the pizzas one at a time. Dip your hands, including the backs of your hands and knuckles, in flour and lift I piece of dough by getting under it with a pastry scraper. Very gently lay the dough across your fists and carefully stretch it by bouncing the dough in a circular motion on your hands, carefully giving it a little stretch with each bounce. If it begins to stick to your hands, lay it down on the floured counter and reflour your hands, then continue shaping it. Once the dough has expanded outward, move to a full toss as shown on page 208. If you have trouble tossing the dough, or if the dough keeps springing back, let it rest for 5 to 20 minutes so the gluten can relax, and try again. You can also resort to using a rolling pin, though this isn't as effective as the toss method.</t>
+  </si>
+  <si>
+    <t>When the dough is stretched out to your satisfaction (about 9 to 12 inches in diameter for a 6-ounce piece of dough), lay it on the peel or pan, making sure there is enough semolina flour or cornmeal to allow it to slide. Lightly top it with sauce and then with your other top- pings, remembering that the best pizzas are topped with a less-is-more philosophy. The American "kitchen sink" approach is counterproductive, as it makes the crust more difficult to bake. A few, usually no more than 3 or 4 toppings, including sauce and cheese is sufficient.</t>
+  </si>
+  <si>
+    <t>Slide the topped pizza onto the stone (or bake directly on the sheet pan) and close the door. Wait 2 minutes, then take a peek. If it needs to be rotated 180 degrees for even baking, do so. The pizza should take about 5 to 8 minutes to bake. If the top gets done before the bottom, you will need to move the stone to a lower self before the next round. if the bottom crisps before the cheese caramelizes, then you will need to raise the stone for subsequent bakes.</t>
+  </si>
+  <si>
+    <t>Remove the pizza from the oven and transfer to a cutting board. Wait 3 to 5 minutes before slicing and serving, to allow the cheese to set slightly</t>
   </si>
 </sst>
 </file>
@@ -761,13 +758,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="12" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFill="1"/>
@@ -778,6 +768,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
@@ -1097,14 +1094,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+    <sheetView tabSelected="1" topLeftCell="A185" workbookViewId="0">
+      <selection activeCell="D207" sqref="D207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="14.44140625" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" customWidth="1"/>
     <col min="3" max="3" width="11" style="2" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" customWidth="1"/>
@@ -1131,72 +1128,72 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7">
+      <c r="A3" s="4">
         <v>35382</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="5">
         <v>100</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="4" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="7">
+      <c r="A4" s="4">
         <v>47024</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="5">
         <v>100</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="7">
+      <c r="A5" s="4">
         <v>47319</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>100</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="7">
+      <c r="A6" s="4">
         <v>54384</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="5">
         <v>100</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="7">
+      <c r="A7" s="4">
         <v>35171</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <v>100</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="6" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1215,59 +1212,59 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="7">
+      <c r="A9" s="4">
         <v>47746</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="5">
         <v>100</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="4" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="7">
+      <c r="A10" s="4">
         <v>47899</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="C10" s="5">
         <v>100</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>161</v>
+      <c r="D10" s="4" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="7">
+      <c r="A11" s="4">
         <v>47042</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="C11" s="5">
         <v>100</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>182</v>
+      <c r="D11" s="6" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="7">
+      <c r="A12" s="4">
         <v>713134</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B12" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="C12" s="5">
         <v>100</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>200</v>
+      <c r="D12" s="4" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1296,663 +1293,663 @@
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="7">
+      <c r="A17" s="4">
         <v>4</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="4">
         <v>35382</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="5">
         <v>2</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7" t="s">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="7">
+      <c r="A18" s="4">
         <v>5</v>
       </c>
-      <c r="B18" s="7">
+      <c r="B18" s="4">
         <v>35382</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="5">
         <v>2</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="7"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="7">
+      <c r="A19" s="4">
         <v>6</v>
       </c>
-      <c r="B19" s="7">
+      <c r="B19" s="4">
         <v>35382</v>
       </c>
-      <c r="C19" s="8">
-        <v>1</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="C19" s="5">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="7" t="s">
+      <c r="F19" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="7">
+      <c r="A20" s="4">
         <v>7</v>
       </c>
-      <c r="B20" s="7">
+      <c r="B20" s="4">
         <v>35382</v>
       </c>
-      <c r="C20" s="8">
+      <c r="C20" s="5">
         <v>2</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="7" t="s">
+      <c r="F20" s="4" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="7">
+      <c r="A21" s="4">
         <v>8</v>
       </c>
-      <c r="B21" s="7">
+      <c r="B21" s="4">
         <v>35382</v>
       </c>
-      <c r="C21" s="8">
+      <c r="C21" s="5">
         <v>0.5</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="7" t="s">
+      <c r="F21" s="4" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="7">
+      <c r="A22" s="4">
         <v>9</v>
       </c>
-      <c r="B22" s="7">
+      <c r="B22" s="4">
         <v>35382</v>
       </c>
-      <c r="C22" s="8">
-        <v>1</v>
-      </c>
-      <c r="D22" s="7" t="s">
+      <c r="C22" s="5">
+        <v>1</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="4" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="7">
+      <c r="A24" s="4">
         <v>0</v>
       </c>
-      <c r="B24" s="7">
+      <c r="B24" s="4">
         <v>47024</v>
       </c>
-      <c r="C24" s="8">
-        <v>1</v>
-      </c>
-      <c r="D24" s="7" t="s">
+      <c r="C24" s="5">
+        <v>1</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="7">
-        <v>1</v>
-      </c>
-      <c r="B25" s="7">
+      <c r="A25" s="4">
+        <v>1</v>
+      </c>
+      <c r="B25" s="4">
         <v>47024</v>
       </c>
-      <c r="C25" s="8">
+      <c r="C25" s="5">
         <v>8</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="E25" s="7" t="s">
+      <c r="E25" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F25" s="7"/>
+      <c r="F25" s="4"/>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="7">
+      <c r="A26" s="4">
         <v>2</v>
       </c>
-      <c r="B26" s="7">
+      <c r="B26" s="4">
         <v>47024</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="7" t="s">
+      <c r="C26" s="5"/>
+      <c r="D26" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F26" s="7"/>
+      <c r="F26" s="4"/>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="7">
+      <c r="A27" s="4">
         <v>3</v>
       </c>
-      <c r="B27" s="7">
+      <c r="B27" s="4">
         <v>47024</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="29" spans="1:6" s="7" customFormat="1">
-      <c r="A29" s="7">
+      <c r="F27" s="4"/>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1">
+      <c r="A29" s="4">
         <v>10</v>
       </c>
-      <c r="B29" s="7">
+      <c r="B29" s="4">
         <v>47319</v>
       </c>
-      <c r="C29" s="8">
+      <c r="C29" s="5">
         <v>12</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="F29" s="7" t="s">
+      <c r="F29" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:6" s="7" customFormat="1">
-      <c r="A30" s="7">
+    <row r="30" spans="1:6" s="4" customFormat="1">
+      <c r="A30" s="4">
         <v>11</v>
       </c>
-      <c r="B30" s="7">
+      <c r="B30" s="4">
         <v>47319</v>
       </c>
-      <c r="C30" s="8">
+      <c r="C30" s="5">
         <v>3</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6" s="7" customFormat="1">
-      <c r="A31" s="7">
+    <row r="31" spans="1:6" s="4" customFormat="1">
+      <c r="A31" s="4">
         <v>12</v>
       </c>
-      <c r="B31" s="7">
+      <c r="B31" s="4">
         <v>47319</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="7" t="s">
+      <c r="C31" s="5"/>
+      <c r="D31" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:6" s="7" customFormat="1">
-      <c r="A32" s="7">
+    <row r="32" spans="1:6" s="4" customFormat="1">
+      <c r="A32" s="4">
         <v>13</v>
       </c>
-      <c r="B32" s="7">
+      <c r="B32" s="4">
         <v>47319</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="7" t="s">
+      <c r="C32" s="5"/>
+      <c r="D32" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="F32" s="7" t="s">
+      <c r="F32" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:6" s="7" customFormat="1">
-      <c r="A33" s="7">
+    <row r="33" spans="1:6" s="4" customFormat="1">
+      <c r="A33" s="4">
         <v>14</v>
       </c>
-      <c r="B33" s="7">
+      <c r="B33" s="4">
         <v>47319</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="7" t="s">
+      <c r="C33" s="5"/>
+      <c r="D33" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F33" s="7" t="s">
+      <c r="F33" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="12" customFormat="1">
-      <c r="C34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" s="7" customFormat="1">
-      <c r="A35" s="7">
+    <row r="34" spans="1:6" s="9" customFormat="1">
+      <c r="C34" s="10"/>
+    </row>
+    <row r="35" spans="1:6" s="4" customFormat="1">
+      <c r="A35" s="4">
         <v>15</v>
       </c>
-      <c r="B35" s="7">
+      <c r="B35" s="4">
         <v>54384</v>
       </c>
-      <c r="C35" s="8">
+      <c r="C35" s="5">
         <v>10</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="E35" s="7" t="s">
+      <c r="E35" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F35" s="7" t="s">
+      <c r="F35" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="7" customFormat="1">
-      <c r="A36" s="7">
+    <row r="36" spans="1:6" s="4" customFormat="1">
+      <c r="A36" s="4">
         <v>16</v>
       </c>
-      <c r="B36" s="7">
+      <c r="B36" s="4">
         <v>54384</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="5">
         <v>2</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F36" s="7" t="s">
+      <c r="F36" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:6" s="7" customFormat="1">
-      <c r="A37" s="7">
+    <row r="37" spans="1:6" s="4" customFormat="1">
+      <c r="A37" s="4">
         <v>17</v>
       </c>
-      <c r="B37" s="7">
+      <c r="B37" s="4">
         <v>54384</v>
       </c>
-      <c r="C37" s="8">
+      <c r="C37" s="5">
         <v>2</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="7" t="s">
+      <c r="F37" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:6" s="7" customFormat="1">
-      <c r="A38" s="7">
+    <row r="38" spans="1:6" s="4" customFormat="1">
+      <c r="A38" s="4">
         <v>18</v>
       </c>
-      <c r="B38" s="7">
+      <c r="B38" s="4">
         <v>54384</v>
       </c>
-      <c r="C38" s="8">
+      <c r="C38" s="5">
         <v>2</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:6" s="7" customFormat="1">
-      <c r="A39" s="7">
+    <row r="39" spans="1:6" s="4" customFormat="1">
+      <c r="A39" s="4">
         <v>19</v>
       </c>
-      <c r="B39" s="7">
+      <c r="B39" s="4">
         <v>54384</v>
       </c>
-      <c r="C39" s="8">
+      <c r="C39" s="5">
         <v>0.33333333333333331</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="F39" s="7" t="s">
+      <c r="F39" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:6" s="7" customFormat="1">
-      <c r="A40" s="7">
+    <row r="40" spans="1:6" s="4" customFormat="1">
+      <c r="A40" s="4">
         <v>20</v>
       </c>
-      <c r="B40" s="7">
+      <c r="B40" s="4">
         <v>54384</v>
       </c>
-      <c r="C40" s="8"/>
-      <c r="D40" s="7" t="s">
+      <c r="C40" s="5"/>
+      <c r="D40" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:6" s="7" customFormat="1">
-      <c r="A41" s="7">
+    <row r="41" spans="1:6" s="4" customFormat="1">
+      <c r="A41" s="4">
         <v>6</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B41" s="4">
         <v>54384</v>
       </c>
-      <c r="C41" s="8">
+      <c r="C41" s="5">
         <v>2</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="E41" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="42" spans="1:6" s="7" customFormat="1">
-      <c r="A42" s="7">
+    <row r="42" spans="1:6" s="4" customFormat="1">
+      <c r="A42" s="4">
         <v>21</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B42" s="4">
         <v>54384</v>
       </c>
-      <c r="C42" s="8">
+      <c r="C42" s="5">
         <v>2</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="E42" s="4" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:6" s="7" customFormat="1">
-      <c r="A43" s="7">
+    <row r="43" spans="1:6" s="4" customFormat="1">
+      <c r="A43" s="4">
         <v>22</v>
       </c>
-      <c r="B43" s="7">
+      <c r="B43" s="4">
         <v>54384</v>
       </c>
-      <c r="C43" s="8">
-        <v>1</v>
-      </c>
-      <c r="D43" s="7" t="s">
+      <c r="C43" s="5">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="44" spans="1:6" s="7" customFormat="1">
-      <c r="A44" s="7">
+    <row r="44" spans="1:6" s="4" customFormat="1">
+      <c r="A44" s="4">
         <v>23</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B44" s="4">
         <v>54384</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="5">
         <v>2</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F44" s="7" t="s">
+      <c r="F44" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="45" spans="1:6" s="7" customFormat="1">
-      <c r="A45" s="7">
+    <row r="45" spans="1:6" s="4" customFormat="1">
+      <c r="A45" s="4">
         <v>17</v>
       </c>
-      <c r="B45" s="7">
+      <c r="B45" s="4">
         <v>54384</v>
       </c>
-      <c r="C45" s="8"/>
-      <c r="D45" s="7" t="s">
+      <c r="C45" s="5"/>
+      <c r="D45" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F45" s="7" t="s">
+      <c r="F45" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="47" spans="1:6" s="7" customFormat="1">
-      <c r="A47" s="7">
+    <row r="47" spans="1:6" s="4" customFormat="1">
+      <c r="A47" s="4">
         <v>24</v>
       </c>
-      <c r="B47" s="7">
+      <c r="B47" s="4">
         <v>35171</v>
       </c>
-      <c r="C47" s="8">
+      <c r="C47" s="5">
         <v>0.25</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F47" s="7" t="s">
+      <c r="F47" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="48" spans="1:6" s="7" customFormat="1">
-      <c r="A48" s="7">
+    <row r="48" spans="1:6" s="4" customFormat="1">
+      <c r="A48" s="4">
         <v>25</v>
       </c>
-      <c r="B48" s="7">
+      <c r="B48" s="4">
         <v>35171</v>
       </c>
-      <c r="C48" s="8">
-        <v>1</v>
-      </c>
-      <c r="D48" s="7" t="s">
+      <c r="C48" s="5">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:6" s="7" customFormat="1">
-      <c r="A49" s="7">
+    <row r="49" spans="1:6" s="4" customFormat="1">
+      <c r="A49" s="4">
         <v>26</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B49" s="4">
         <v>35171</v>
       </c>
-      <c r="C49" s="8">
+      <c r="C49" s="5">
         <v>0.5</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F49" s="7" t="s">
+      <c r="F49" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="7" customFormat="1">
-      <c r="A50" s="7">
+    <row r="50" spans="1:6" s="4" customFormat="1">
+      <c r="A50" s="4">
         <v>27</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B50" s="4">
         <v>35171</v>
       </c>
-      <c r="C50" s="8">
-        <v>1</v>
-      </c>
-      <c r="D50" s="7" t="s">
+      <c r="C50" s="5">
+        <v>1</v>
+      </c>
+      <c r="D50" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F50" s="7" t="s">
+      <c r="F50" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:6" s="7" customFormat="1">
-      <c r="A51" s="7">
+    <row r="51" spans="1:6" s="4" customFormat="1">
+      <c r="A51" s="4">
         <v>28</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B51" s="4">
         <v>35171</v>
       </c>
-      <c r="C51" s="8">
-        <v>1</v>
-      </c>
-      <c r="D51" s="7" t="s">
+      <c r="C51" s="5">
+        <v>1</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F51" s="7" t="s">
+      <c r="F51" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:6" s="7" customFormat="1">
-      <c r="A52" s="7">
+    <row r="52" spans="1:6" s="4" customFormat="1">
+      <c r="A52" s="4">
         <v>29</v>
       </c>
-      <c r="B52" s="7">
+      <c r="B52" s="4">
         <v>35171</v>
       </c>
-      <c r="C52" s="8">
-        <v>1</v>
-      </c>
-      <c r="D52" s="7" t="s">
+      <c r="C52" s="5">
+        <v>1</v>
+      </c>
+      <c r="D52" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F52" s="7" t="s">
+      <c r="F52" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:6" s="7" customFormat="1">
-      <c r="A53" s="7">
+    <row r="53" spans="1:6" s="4" customFormat="1">
+      <c r="A53" s="4">
         <v>30</v>
       </c>
-      <c r="B53" s="7">
+      <c r="B53" s="4">
         <v>35171</v>
       </c>
-      <c r="C53" s="8">
-        <v>1</v>
-      </c>
-      <c r="D53" s="7" t="s">
+      <c r="C53" s="5">
+        <v>1</v>
+      </c>
+      <c r="D53" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="E53" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F53" s="7" t="s">
+      <c r="F53" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:6" s="7" customFormat="1">
-      <c r="A54" s="7">
+    <row r="54" spans="1:6" s="4" customFormat="1">
+      <c r="A54" s="4">
         <v>8</v>
       </c>
-      <c r="B54" s="7">
+      <c r="B54" s="4">
         <v>35171</v>
       </c>
-      <c r="C54" s="8">
+      <c r="C54" s="5">
         <v>0.5</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E54" s="7" t="s">
+      <c r="E54" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F54" s="7" t="s">
+      <c r="F54" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:6" s="7" customFormat="1">
-      <c r="A55" s="7">
+    <row r="55" spans="1:6" s="4" customFormat="1">
+      <c r="A55" s="4">
         <v>31</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B55" s="4">
         <v>35171</v>
       </c>
-      <c r="C55" s="8">
+      <c r="C55" s="5">
         <v>2</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="E55" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:6" s="7" customFormat="1">
-      <c r="A56" s="7">
+    <row r="56" spans="1:6" s="4" customFormat="1">
+      <c r="A56" s="4">
         <v>6</v>
       </c>
-      <c r="B56" s="7">
+      <c r="B56" s="4">
         <v>35171</v>
       </c>
-      <c r="C56" s="8">
-        <v>1</v>
-      </c>
-      <c r="D56" s="7" t="s">
+      <c r="C56" s="5">
+        <v>1</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E56" s="7" t="s">
+      <c r="E56" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F56" s="7" t="s">
+      <c r="F56" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2013,6 +2010,9 @@
       </c>
     </row>
     <row r="62" spans="1:6">
+      <c r="A62">
+        <v>21</v>
+      </c>
       <c r="B62" t="s">
         <v>111</v>
       </c>
@@ -2054,7 +2054,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="2:6">
+    <row r="65" spans="1:6">
       <c r="B65" t="s">
         <v>111</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="2:6">
+    <row r="66" spans="1:6">
       <c r="B66" t="s">
         <v>111</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="67" spans="2:6">
+    <row r="67" spans="1:6">
       <c r="B67" t="s">
         <v>111</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="2:6">
+    <row r="68" spans="1:6">
       <c r="B68" t="s">
         <v>111</v>
       </c>
@@ -2104,7 +2104,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="2:6">
+    <row r="69" spans="1:6">
       <c r="B69" t="s">
         <v>111</v>
       </c>
@@ -2112,7 +2112,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="2:6">
+    <row r="70" spans="1:6">
       <c r="B70" t="s">
         <v>111</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="71" spans="2:6">
+    <row r="71" spans="1:6">
       <c r="B71" t="s">
         <v>111</v>
       </c>
@@ -2140,7 +2140,10 @@
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="2:6">
+    <row r="72" spans="1:6">
+      <c r="A72">
+        <v>22</v>
+      </c>
       <c r="B72" t="s">
         <v>111</v>
       </c>
@@ -2154,7 +2157,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="73" spans="2:6">
+    <row r="73" spans="1:6">
       <c r="B73" t="s">
         <v>111</v>
       </c>
@@ -2168,7 +2171,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="74" spans="2:6">
+    <row r="74" spans="1:6">
       <c r="B74" t="s">
         <v>111</v>
       </c>
@@ -2182,7 +2185,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="75" spans="2:6">
+    <row r="75" spans="1:6">
       <c r="B75" t="s">
         <v>111</v>
       </c>
@@ -2196,412 +2199,463 @@
         <v>128</v>
       </c>
     </row>
-    <row r="77" spans="2:6">
-      <c r="B77">
+    <row r="77" spans="1:6" s="4" customFormat="1">
+      <c r="A77" s="4">
+        <v>21</v>
+      </c>
+      <c r="B77" s="4">
         <v>47746</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="C77" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D77" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="E77" t="s">
+      <c r="E77" s="4" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="78" spans="2:6">
-      <c r="B78">
+    <row r="78" spans="1:6" s="4" customFormat="1">
+      <c r="A78" s="4">
+        <v>32</v>
+      </c>
+      <c r="B78" s="4">
         <v>47746</v>
       </c>
-      <c r="C78" s="2" t="s">
+      <c r="C78" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D78" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E78" t="s">
+      <c r="E78" s="4" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="79" spans="2:6">
-      <c r="B79">
+    <row r="79" spans="1:6" s="4" customFormat="1">
+      <c r="A79" s="4">
+        <v>33</v>
+      </c>
+      <c r="B79" s="4">
         <v>47746</v>
       </c>
-      <c r="C79" s="2">
-        <v>1</v>
-      </c>
-      <c r="D79" t="s">
+      <c r="C79" s="5">
+        <v>1</v>
+      </c>
+      <c r="D79" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E79" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="2:6">
-      <c r="B80">
+    <row r="80" spans="1:6" s="4" customFormat="1">
+      <c r="A80" s="4">
+        <v>11</v>
+      </c>
+      <c r="B80" s="4">
         <v>47746</v>
       </c>
-      <c r="C80" s="2">
+      <c r="C80" s="5">
         <v>0.25</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D80" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="E80" t="s">
+      <c r="E80" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F80" t="s">
+      <c r="F80" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="2:6">
-      <c r="B81">
+    <row r="81" spans="1:6" s="4" customFormat="1">
+      <c r="A81" s="4">
+        <v>1</v>
+      </c>
+      <c r="B81" s="4">
         <v>47746</v>
       </c>
-      <c r="C81" s="2" t="s">
+      <c r="C81" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D81" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E81" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F81" t="s">
+      <c r="F81" s="4" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="82" spans="2:6">
-      <c r="B82">
+    <row r="82" spans="1:6" s="4" customFormat="1">
+      <c r="A82" s="4">
+        <v>35</v>
+      </c>
+      <c r="B82" s="4">
         <v>47746</v>
       </c>
-      <c r="D82" t="s">
+      <c r="C82" s="5"/>
+      <c r="D82" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F82" t="s">
+      <c r="F82" s="4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="84" spans="2:6">
-      <c r="B84">
+    <row r="84" spans="1:6" s="4" customFormat="1">
+      <c r="A84" s="4">
+        <v>11</v>
+      </c>
+      <c r="B84" s="4">
         <v>47899</v>
       </c>
-      <c r="C84" s="2">
+      <c r="C84" s="5">
         <v>0.5</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D84" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" s="4" customFormat="1">
+      <c r="A85" s="4">
+        <v>14</v>
+      </c>
+      <c r="B85" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C85" s="5">
+        <v>1</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" s="4" customFormat="1">
+      <c r="A86" s="4">
+        <v>36</v>
+      </c>
+      <c r="B86" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C86" s="5">
+        <v>1</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" s="4" customFormat="1">
+      <c r="A87" s="4">
+        <v>37</v>
+      </c>
+      <c r="B87" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C87" s="5">
+        <v>1</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" s="4" customFormat="1">
+      <c r="A88" s="4">
+        <v>38</v>
+      </c>
+      <c r="B88" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C88" s="5">
+        <v>2</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" s="4" customFormat="1">
+      <c r="A89" s="4">
+        <v>16</v>
+      </c>
+      <c r="B89" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C89" s="5">
+        <v>2</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" s="4" customFormat="1">
+      <c r="A90" s="4">
+        <v>39</v>
+      </c>
+      <c r="B90" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C90" s="5">
+        <v>1</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" s="4" customFormat="1">
+      <c r="A91" s="4">
+        <v>40</v>
+      </c>
+      <c r="B91" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" s="4" customFormat="1">
+      <c r="A92" s="4">
+        <v>41</v>
+      </c>
+      <c r="B92" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C92" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="D92" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" s="4" customFormat="1">
+      <c r="A93" s="4">
+        <v>42</v>
+      </c>
+      <c r="B93" s="4">
+        <v>47899</v>
+      </c>
+      <c r="C93" s="5">
+        <v>1</v>
+      </c>
+      <c r="D93" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="E84" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6">
-      <c r="B85">
-        <v>47899</v>
-      </c>
-      <c r="C85" s="2">
-        <v>1</v>
-      </c>
-      <c r="D85" t="s">
-        <v>163</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="E93" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" s="4" customFormat="1">
+      <c r="B95" s="4">
+        <v>47042</v>
+      </c>
+      <c r="C95" s="5">
+        <v>1</v>
+      </c>
+      <c r="D95" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" s="4" customFormat="1">
+      <c r="B96" s="4">
+        <v>47042</v>
+      </c>
+      <c r="C96" s="5">
+        <v>1</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" s="4" customFormat="1">
+      <c r="B97" s="4">
+        <v>47042</v>
+      </c>
+      <c r="C97" s="5">
+        <v>1</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" s="4" customFormat="1">
+      <c r="B98" s="4">
+        <v>47042</v>
+      </c>
+      <c r="C98" s="5">
+        <v>2</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" s="4" customFormat="1">
+      <c r="B99" s="4">
+        <v>47042</v>
+      </c>
+      <c r="C99" s="5">
+        <v>2</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" s="4" customFormat="1" ht="13.8" customHeight="1">
+      <c r="B100" s="4">
+        <v>47042</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" s="4" customFormat="1">
+      <c r="B102" s="4">
+        <v>713134</v>
+      </c>
+      <c r="C102" s="5">
+        <v>4</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" s="4" customFormat="1">
+      <c r="B103" s="4">
+        <v>713134</v>
+      </c>
+      <c r="C103" s="5">
+        <v>3</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" s="4" customFormat="1">
+      <c r="B104" s="4">
+        <v>713134</v>
+      </c>
+      <c r="C104" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="E104" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="86" spans="2:6">
-      <c r="B86">
-        <v>47899</v>
-      </c>
-      <c r="C86" s="2">
-        <v>1</v>
-      </c>
-      <c r="D86" t="s">
-        <v>164</v>
-      </c>
-      <c r="E86" t="s">
+    <row r="105" spans="2:6" s="4" customFormat="1">
+      <c r="B105" s="4">
+        <v>713134</v>
+      </c>
+      <c r="C105" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E105" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="87" spans="2:6">
-      <c r="B87">
-        <v>47899</v>
-      </c>
-      <c r="C87" s="2">
-        <v>1</v>
-      </c>
-      <c r="D87" t="s">
-        <v>165</v>
-      </c>
-      <c r="E87" t="s">
+    <row r="106" spans="2:6" s="4" customFormat="1">
+      <c r="B106" s="4">
+        <v>713134</v>
+      </c>
+      <c r="C106" s="5">
+        <v>2</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="E106" s="4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="88" spans="2:6">
-      <c r="B88">
-        <v>47899</v>
-      </c>
-      <c r="C88" s="2">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s">
-        <v>174</v>
-      </c>
-      <c r="E88" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6">
-      <c r="B89">
-        <v>47899</v>
-      </c>
-      <c r="C89" s="2">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s">
-        <v>171</v>
-      </c>
-      <c r="F89" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6">
-      <c r="B90">
-        <v>47899</v>
-      </c>
-      <c r="C90" s="2">
-        <v>1</v>
-      </c>
-      <c r="D90" t="s">
-        <v>167</v>
-      </c>
-      <c r="F90" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6">
-      <c r="B91">
-        <v>47899</v>
-      </c>
-      <c r="D91" t="s">
-        <v>168</v>
-      </c>
-      <c r="E91" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6">
-      <c r="B92">
-        <v>47899</v>
-      </c>
-      <c r="C92" s="2">
-        <v>0.25</v>
-      </c>
-      <c r="D92" t="s">
-        <v>169</v>
-      </c>
-      <c r="E92" t="s">
+    <row r="107" spans="2:6" s="4" customFormat="1">
+      <c r="B107" s="4">
+        <v>713134</v>
+      </c>
+      <c r="C107" s="5">
+        <v>1</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="E107" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F92" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6">
-      <c r="B93">
-        <v>47899</v>
-      </c>
-      <c r="C93" s="2">
-        <v>1</v>
-      </c>
-      <c r="D93" t="s">
-        <v>170</v>
-      </c>
-      <c r="E93" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="95" spans="2:6">
-      <c r="B95">
-        <v>47042</v>
-      </c>
-      <c r="C95" s="2">
-        <v>1</v>
-      </c>
-      <c r="D95" t="s">
-        <v>183</v>
-      </c>
-      <c r="E95" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="96" spans="2:6">
-      <c r="B96">
-        <v>47042</v>
-      </c>
-      <c r="C96" s="2">
-        <v>1</v>
-      </c>
-      <c r="D96" t="s">
-        <v>184</v>
-      </c>
-      <c r="E96" t="s">
-        <v>57</v>
-      </c>
-      <c r="F96" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="97" spans="2:6">
-      <c r="B97">
-        <v>47042</v>
-      </c>
-      <c r="C97" s="2">
-        <v>1</v>
-      </c>
-      <c r="D97" t="s">
-        <v>187</v>
-      </c>
-      <c r="E97" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="98" spans="2:6">
-      <c r="B98">
-        <v>47042</v>
-      </c>
-      <c r="C98" s="2">
-        <v>2</v>
-      </c>
-      <c r="D98" t="s">
-        <v>190</v>
-      </c>
-      <c r="E98" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="99" spans="2:6">
-      <c r="B99">
-        <v>47042</v>
-      </c>
-      <c r="C99" s="2">
-        <v>2</v>
-      </c>
-      <c r="D99" t="s">
-        <v>189</v>
-      </c>
-      <c r="E99" t="s">
+    </row>
+    <row r="108" spans="2:6" s="4" customFormat="1">
+      <c r="B108" s="4">
+        <v>713134</v>
+      </c>
+      <c r="C108" s="5">
+        <v>4</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="E108" s="4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="100" spans="2:6">
-      <c r="B100">
-        <v>47042</v>
-      </c>
-      <c r="D100" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="102" spans="2:6">
-      <c r="B102">
-        <v>713134</v>
-      </c>
-      <c r="C102" s="2">
-        <v>4</v>
-      </c>
-      <c r="D102" t="s">
-        <v>201</v>
-      </c>
-      <c r="E102" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="103" spans="2:6">
-      <c r="B103">
-        <v>713134</v>
-      </c>
-      <c r="C103" s="2">
-        <v>3</v>
-      </c>
-      <c r="D103" t="s">
-        <v>202</v>
-      </c>
-      <c r="E103" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="104" spans="2:6">
-      <c r="B104">
-        <v>713134</v>
-      </c>
-      <c r="C104" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D104" t="s">
-        <v>203</v>
-      </c>
-      <c r="E104" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="105" spans="2:6">
-      <c r="B105">
-        <v>713134</v>
-      </c>
-      <c r="C105" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="D105" t="s">
-        <v>120</v>
-      </c>
-      <c r="E105" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="106" spans="2:6">
-      <c r="B106">
-        <v>713134</v>
-      </c>
-      <c r="C106" s="2">
-        <v>2</v>
-      </c>
-      <c r="D106" t="s">
-        <v>166</v>
-      </c>
-      <c r="E106" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="107" spans="2:6">
-      <c r="B107">
-        <v>713134</v>
-      </c>
-      <c r="C107" s="2">
-        <v>1</v>
-      </c>
-      <c r="D107" t="s">
-        <v>204</v>
-      </c>
-      <c r="E107" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="108" spans="2:6">
-      <c r="B108">
-        <v>713134</v>
-      </c>
-      <c r="C108" s="2">
-        <v>4</v>
-      </c>
-      <c r="D108" t="s">
-        <v>205</v>
-      </c>
-      <c r="E108" t="s">
-        <v>84</v>
-      </c>
-      <c r="F108" t="s">
+      <c r="F108" s="4" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2640,272 +2694,272 @@
         <v>15</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="27.6">
-      <c r="A136" s="7">
+    <row r="136" spans="1:3" ht="124.2">
+      <c r="A136" s="4">
         <v>35382</v>
       </c>
-      <c r="B136" s="10" t="s">
+      <c r="B136" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C136" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137" spans="1:3" ht="55.2">
-      <c r="A137" s="7">
+      <c r="C136" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" ht="220.8">
+      <c r="A137" s="4">
         <v>35382</v>
       </c>
-      <c r="B137" s="10" t="s">
+      <c r="B137" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C137" s="8">
+      <c r="C137" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:3" ht="55.2">
-      <c r="A138" s="7">
+    <row r="138" spans="1:3" ht="220.8">
+      <c r="A138" s="4">
         <v>35382</v>
       </c>
-      <c r="B138" s="10" t="s">
+      <c r="B138" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C138" s="8">
+      <c r="C138" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="27.6">
-      <c r="A139" s="7">
+    <row r="139" spans="1:3" ht="124.2">
+      <c r="A139" s="4">
         <v>35382</v>
       </c>
-      <c r="B139" s="10" t="s">
+      <c r="B139" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C139" s="8">
+      <c r="C139" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="96.6">
-      <c r="A140" s="7">
+    <row r="140" spans="1:3" ht="400.2">
+      <c r="A140" s="4">
         <v>35382</v>
       </c>
-      <c r="B140" s="10" t="s">
+      <c r="B140" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C140" s="8">
+      <c r="C140" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="27.6">
-      <c r="A141" s="7">
+    <row r="141" spans="1:3" ht="69">
+      <c r="A141" s="4">
         <v>35382</v>
       </c>
-      <c r="B141" s="10" t="s">
+      <c r="B141" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C141" s="8">
+      <c r="C141" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="41.4">
-      <c r="A142" s="7">
+    <row r="142" spans="1:3" ht="165.6">
+      <c r="A142" s="4">
         <v>35382</v>
       </c>
-      <c r="B142" s="10" t="s">
+      <c r="B142" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C142" s="8">
+      <c r="C142" s="5">
         <v>7</v>
       </c>
     </row>
     <row r="143" spans="1:3">
-      <c r="A143" s="7"/>
-      <c r="B143" s="7"/>
-      <c r="C143" s="8"/>
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="5"/>
     </row>
     <row r="144" spans="1:3" ht="15.6">
-      <c r="A144" s="7">
+      <c r="A144" s="4">
         <v>47024</v>
       </c>
-      <c r="B144" s="11" t="s">
+      <c r="B144" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C144" s="8">
+      <c r="C144" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:3" ht="15.6">
-      <c r="A145" s="7">
+      <c r="A145" s="4">
         <v>47024</v>
       </c>
-      <c r="B145" s="11" t="s">
+      <c r="B145" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="C145" s="8">
+      <c r="C145" s="5">
         <v>2</v>
       </c>
     </row>
     <row r="146" spans="1:3" ht="15.6">
-      <c r="A146" s="7">
+      <c r="A146" s="4">
         <v>47024</v>
       </c>
-      <c r="B146" s="11" t="s">
+      <c r="B146" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="C146" s="8">
+      <c r="C146" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="15.6">
-      <c r="A147" s="7">
+      <c r="A147" s="4">
         <v>47024</v>
       </c>
-      <c r="B147" s="11" t="s">
+      <c r="B147" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C147" s="8">
+      <c r="C147" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:3" s="7" customFormat="1" ht="15.6">
-      <c r="A149" s="7">
+    <row r="149" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A149" s="4">
         <v>47319</v>
       </c>
-      <c r="B149" s="11" t="s">
+      <c r="B149" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="C149" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150" spans="1:3" s="7" customFormat="1" ht="15.6">
-      <c r="A150" s="7">
+      <c r="C149" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A150" s="4">
         <v>47319</v>
       </c>
-      <c r="B150" s="11" t="s">
+      <c r="B150" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C150" s="8">
+      <c r="C150" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:3" s="7" customFormat="1" ht="15.6">
-      <c r="A151" s="7">
+    <row r="151" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A151" s="4">
         <v>47319</v>
       </c>
-      <c r="B151" s="11" t="s">
+      <c r="B151" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C151" s="8">
+      <c r="C151" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="152" spans="1:3" s="7" customFormat="1" ht="15.6">
-      <c r="A152" s="7">
+    <row r="152" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A152" s="4">
         <v>47319</v>
       </c>
-      <c r="B152" s="11" t="s">
+      <c r="B152" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="C152" s="8">
+      <c r="C152" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:3" s="7" customFormat="1" ht="15.6">
-      <c r="A153" s="7">
+    <row r="153" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A153" s="4">
         <v>47319</v>
       </c>
-      <c r="B153" s="11" t="s">
+      <c r="B153" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C153" s="8">
+      <c r="C153" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="155" spans="1:3" s="7" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A155" s="7">
+    <row r="155" spans="1:3" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A155" s="4">
         <v>54384</v>
       </c>
-      <c r="B155" s="14" t="s">
+      <c r="B155" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="C155" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" s="7" customFormat="1" ht="13.5" customHeight="1">
-      <c r="A156" s="7">
+      <c r="C155" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A156" s="4">
         <v>54384</v>
       </c>
-      <c r="B156" s="14" t="s">
+      <c r="B156" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C156" s="8">
+      <c r="C156" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:3" s="7" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A157" s="7">
+    <row r="157" spans="1:3" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A157" s="4">
         <v>54384</v>
       </c>
-      <c r="B157" s="14" t="s">
+      <c r="B157" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="C157" s="8">
+      <c r="C157" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="158" spans="1:3" s="7" customFormat="1" ht="20.25" customHeight="1">
-      <c r="A158" s="7">
+    <row r="158" spans="1:3" s="4" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A158" s="4">
         <v>54384</v>
       </c>
-      <c r="B158" s="14" t="s">
+      <c r="B158" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="C158" s="8">
+      <c r="C158" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:3" s="7" customFormat="1" ht="41.4">
-      <c r="A160" s="7">
+    <row r="160" spans="1:3" s="4" customFormat="1" ht="124.2">
+      <c r="A160" s="4">
         <v>35171</v>
       </c>
-      <c r="B160" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="C160" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" s="7" customFormat="1" ht="82.8">
-      <c r="A161" s="7">
+      <c r="B160" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="C160" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" s="4" customFormat="1" ht="303.60000000000002">
+      <c r="A161" s="4">
         <v>35171</v>
       </c>
-      <c r="B161" s="10" t="s">
-        <v>213</v>
-      </c>
-      <c r="C161" s="8">
+      <c r="B161" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C161" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" s="7" customFormat="1" ht="27.6">
-      <c r="A162" s="7">
+    <row r="162" spans="1:3" s="4" customFormat="1" ht="69">
+      <c r="A162" s="4">
         <v>35171</v>
       </c>
-      <c r="B162" s="10" t="s">
-        <v>212</v>
-      </c>
-      <c r="C162" s="8">
+      <c r="B162" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C162" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="163" spans="1:3" s="7" customFormat="1" ht="41.4">
-      <c r="A163" s="7">
+    <row r="163" spans="1:3" s="4" customFormat="1" ht="165.6">
+      <c r="A163" s="4">
         <v>35171</v>
       </c>
-      <c r="B163" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="C163" s="8">
+      <c r="B163" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C163" s="5">
         <v>4</v>
       </c>
     </row>
@@ -3020,278 +3074,276 @@
       </c>
     </row>
     <row r="175" spans="1:3" ht="15" customHeight="1"/>
-    <row r="176" spans="1:3" ht="409.6">
-      <c r="A176">
+    <row r="176" spans="1:3" s="4" customFormat="1">
+      <c r="A176" s="4">
         <v>47746</v>
       </c>
-      <c r="B176" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="C176" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A177">
+      <c r="B176" s="12"/>
+      <c r="C176" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" s="4" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A177" s="4">
         <v>47746</v>
       </c>
-      <c r="B177" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C177" s="2">
+      <c r="B177" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C177" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="178" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A178">
+    <row r="178" spans="1:3" s="4" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A178" s="4">
         <v>47746</v>
       </c>
-      <c r="B178" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C178" s="2">
+      <c r="B178" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C178" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A179">
+    <row r="179" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A179" s="4">
         <v>47746</v>
       </c>
-      <c r="B179" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="C179" s="2">
+      <c r="B179" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="C179" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A180">
+    <row r="180" spans="1:3" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A180" s="4">
         <v>47746</v>
       </c>
-      <c r="B180" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C180" s="2">
+      <c r="B180" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="C180" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A181">
+    <row r="181" spans="1:3" s="4" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A181" s="4">
         <v>47746</v>
       </c>
-      <c r="B181" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C181" s="2">
+      <c r="B181" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="C181" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="182" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A182">
+    <row r="182" spans="1:3" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A182" s="4">
         <v>47746</v>
       </c>
-      <c r="B182" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C182" s="2">
+      <c r="B182" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C182" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="183" spans="1:3" ht="13.5" customHeight="1">
-      <c r="A183">
+    <row r="183" spans="1:3" s="4" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A183" s="4">
         <v>47746</v>
       </c>
-      <c r="B183" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C183" s="2">
+      <c r="B183" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C183" s="5">
         <v>8</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A184">
+    <row r="184" spans="1:3" s="4" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A184" s="4">
         <v>47746</v>
       </c>
-      <c r="B184" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C184" s="2">
+      <c r="B184" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C184" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="186" spans="1:3">
-      <c r="A186">
+    <row r="186" spans="1:3" s="4" customFormat="1">
+      <c r="A186" s="4">
         <v>47899</v>
       </c>
-      <c r="B186" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="C186" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187">
+      <c r="B186" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C186" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" s="4" customFormat="1">
+      <c r="A187" s="4">
         <v>47899</v>
       </c>
-      <c r="B187" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C187" s="2">
+      <c r="B187" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C187" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="188" spans="1:3">
-      <c r="A188">
+    <row r="188" spans="1:3" s="4" customFormat="1">
+      <c r="A188" s="4">
         <v>47899</v>
       </c>
-      <c r="B188" s="5" t="s">
-        <v>179</v>
-      </c>
-      <c r="C188" s="2">
+      <c r="B188" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C188" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="189" spans="1:3">
-      <c r="A189">
+    <row r="189" spans="1:3" s="4" customFormat="1">
+      <c r="A189" s="4">
         <v>47899</v>
       </c>
-      <c r="B189" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="C189" s="2">
+      <c r="B189" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="C189" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="15.6">
-      <c r="A191">
+    <row r="191" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A191" s="4">
         <v>47042</v>
       </c>
-      <c r="B191" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="C191" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" ht="15.6">
-      <c r="A192">
+      <c r="B191" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="C191" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A192" s="4">
         <v>47042</v>
       </c>
-      <c r="B192" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="C192" s="2">
+      <c r="B192" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="C192" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:3" ht="15.6">
-      <c r="A193">
+    <row r="193" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A193" s="4">
         <v>47042</v>
       </c>
-      <c r="B193" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="C193" s="2">
+      <c r="B193" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="C193" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="15.6">
-      <c r="A194">
+    <row r="194" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A194" s="4">
         <v>47042</v>
       </c>
-      <c r="B194" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="C194" s="2">
+      <c r="B194" s="8" t="s">
+        <v>187</v>
+      </c>
+      <c r="C194" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="15.6">
-      <c r="A195">
+    <row r="195" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A195" s="4">
         <v>47042</v>
       </c>
-      <c r="B195" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="C195" s="2">
+      <c r="B195" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C195" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="15.6">
-      <c r="A196">
+    <row r="196" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A196" s="4">
         <v>47042</v>
       </c>
-      <c r="B196" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="C196" s="2">
+      <c r="B196" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="C196" s="5">
         <v>6</v>
       </c>
     </row>
-    <row r="197" spans="1:3" ht="15.6">
-      <c r="A197">
+    <row r="197" spans="1:3" s="4" customFormat="1" ht="15.6">
+      <c r="A197" s="4">
         <v>47042</v>
       </c>
-      <c r="B197" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="C197" s="2">
+      <c r="B197" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C197" s="5">
         <v>7</v>
       </c>
     </row>
-    <row r="199" spans="1:3">
-      <c r="A199">
+    <row r="199" spans="1:3" s="4" customFormat="1" ht="27.6">
+      <c r="A199" s="4">
         <v>713134</v>
       </c>
-      <c r="B199" s="6" t="s">
+      <c r="B199" s="14" t="s">
+        <v>202</v>
+      </c>
+      <c r="C199" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A200" s="4">
+        <v>713134</v>
+      </c>
+      <c r="B200" s="14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C200" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" s="4" customFormat="1" ht="16.5" customHeight="1">
+      <c r="A201" s="4">
+        <v>713134</v>
+      </c>
+      <c r="B201" s="14" t="s">
+        <v>204</v>
+      </c>
+      <c r="C201" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" s="4" customFormat="1" ht="17.25" customHeight="1">
+      <c r="A202" s="4">
+        <v>713134</v>
+      </c>
+      <c r="B202" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="C202" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" s="4" customFormat="1" ht="15.75" customHeight="1">
+      <c r="A203" s="4">
+        <v>713134</v>
+      </c>
+      <c r="B203" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="C199" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="200" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A200">
-        <v>713134</v>
-      </c>
-      <c r="B200" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C200" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="201" spans="1:3" ht="16.5" customHeight="1">
-      <c r="A201">
-        <v>713134</v>
-      </c>
-      <c r="B201" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="C201" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" ht="17.25" customHeight="1">
-      <c r="A202">
-        <v>713134</v>
-      </c>
-      <c r="B202" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="C202" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="203" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A203">
-        <v>713134</v>
-      </c>
-      <c r="B203" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C203" s="2">
+      <c r="C203" s="5">
         <v>5</v>
       </c>
     </row>

</xml_diff>